<commit_message>
updated data for kli
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -156,9 +156,6 @@
     <t>CoverageAmount</t>
   </si>
   <si>
-    <t>Annual Income</t>
-  </si>
-  <si>
     <t>Qualification</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>//*[@class="long-value-input qualification"]</t>
   </si>
   <si>
-    <t>Post-graduate Master’s degree, PHD</t>
-  </si>
-  <si>
     <t>//*[contains(text(),'Get Kotak Life Discount')]</t>
   </si>
   <si>
@@ -238,6 +232,36 @@
   </si>
   <si>
     <t>PROCEEDTOCUSTOMIZE</t>
+  </si>
+  <si>
+    <t>AnnualIncomePopUp</t>
+  </si>
+  <si>
+    <t>//input[@name='annual_income']</t>
+  </si>
+  <si>
+    <t>AnnualIncome</t>
+  </si>
+  <si>
+    <t>10,00,000</t>
+  </si>
+  <si>
+    <t>//*[@class="popup-main-btn"]</t>
+  </si>
+  <si>
+    <t>PGQualification</t>
+  </si>
+  <si>
+    <t>CSS = button[type='submit']</t>
+  </si>
+  <si>
+    <t>AnnualIncomeDone</t>
+  </si>
+  <si>
+    <t>QualificationDone</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
   </si>
 </sst>
 </file>
@@ -247,7 +271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,16 +291,6 @@
       <u/>
       <sz val="10"/>
       <color indexed="12"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -316,28 +330,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF757575"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF757575"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -514,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -527,47 +519,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -575,7 +531,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -601,24 +557,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1317,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,29 +1314,29 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="30" t="s">
         <v>24</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J1" s="5"/>
-      <c r="K1" s="14"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1379,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>28</v>
@@ -1388,7 +1359,7 @@
         <v>29</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>30</v>
@@ -1412,10 +1383,10 @@
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1424,17 +1395,17 @@
       <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="46">
+      <c r="G4" s="32">
         <v>9999999999</v>
       </c>
-      <c r="H4" s="50" t="s">
-        <v>48</v>
+      <c r="H4" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>3</v>
@@ -1443,8 +1414,8 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1456,8 +1427,8 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1469,7 +1440,7 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1482,7 +1453,7 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1490,25 +1461,25 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="25"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="26"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1521,7 +1492,7 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1534,7 +1505,7 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1547,7 +1518,7 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1587,7 +1558,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E2" sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,81 +1567,116 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="7" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="H1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="H2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>101</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>25000000</v>
       </c>
-      <c r="D4" s="46">
-        <v>1000000</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1683,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,474 +1727,457 @@
     <col min="34" max="34" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AH1" s="3"/>
+    </row>
+    <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" s="46" t="s">
+      <c r="D2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="4"/>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="4"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AH2" s="3"/>
+    </row>
+    <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+    </row>
+    <row r="4" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>101</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="3">
         <v>1974551</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="4"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AG7" s="4"/>
-      <c r="AH7" s="4"/>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4"/>
-      <c r="AG9" s="4"/>
-      <c r="AH9" s="4"/>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="22"/>
-      <c r="K10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AC10" s="17"/>
-    </row>
-    <row r="11" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="18"/>
-      <c r="U11" s="18"/>
-      <c r="V11" s="21"/>
-      <c r="W11" s="18"/>
-      <c r="X11" s="18"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="4"/>
-      <c r="AG11" s="4"/>
-      <c r="AH11" s="4"/>
-    </row>
-    <row r="12" spans="1:34" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
-      <c r="U12" s="18"/>
-      <c r="V12" s="21"/>
-      <c r="W12" s="18"/>
-      <c r="X12" s="18"/>
-      <c r="Y12" s="18"/>
-      <c r="Z12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
-      <c r="AE12" s="18"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
-      <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="4"/>
-      <c r="AG13" s="4"/>
-      <c r="AH13" s="4"/>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="4"/>
-      <c r="E14" s="22"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+    </row>
+    <row r="5" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+    </row>
+    <row r="6" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="35"/>
+      <c r="R6" s="35"/>
+      <c r="S6" s="35"/>
+      <c r="T6" s="35"/>
+      <c r="U6" s="35"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="37"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+    </row>
+    <row r="7" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="35"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+    </row>
+    <row r="8" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="V8" s="39"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+    </row>
+    <row r="9" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="V9" s="39"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+    </row>
+    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="V10" s="39"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AC10" s="40"/>
+    </row>
+    <row r="11" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="42"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="41"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="41"/>
+      <c r="AD11" s="41"/>
+      <c r="AE11" s="41"/>
+      <c r="AF11" s="3"/>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+    </row>
+    <row r="12" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="41"/>
+      <c r="AB12" s="41"/>
+      <c r="AC12" s="41"/>
+      <c r="AD12" s="41"/>
+      <c r="AE12" s="41"/>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+    </row>
+    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+    </row>
+    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2299,10 +2288,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2310,10 +2299,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
         <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2343,11 +2332,11 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2404,52 +2393,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>59</v>
+      <c r="C1" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="31"/>
+        <v>52</v>
+      </c>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="17"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -2457,10 +2446,10 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2516,82 +2505,82 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="16"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="37"/>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="37"/>
-      <c r="AG4" s="37"/>
-      <c r="AH4" s="37"/>
-      <c r="AI4" s="37"/>
-      <c r="AJ4" s="37"/>
-      <c r="AK4" s="37"/>
-      <c r="AL4" s="38"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="23"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="24"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="29"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="5"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="29"/>
-      <c r="U5" s="29"/>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="29"/>
-      <c r="AG5" s="29"/>
-      <c r="AH5" s="29"/>
-      <c r="AI5" s="29"/>
-      <c r="AJ5" s="29"/>
-      <c r="AK5" s="29"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
       <c r="AL5" s="5"/>
     </row>
   </sheetData>
@@ -2614,161 +2603,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="41">
+      <c r="A4" s="27">
         <v>111</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="27">
         <v>1</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="27">
         <v>0</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2854,7 +2843,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="39">
+      <c r="A7" s="25">
         <v>106</v>
       </c>
       <c r="B7" s="3">

</xml_diff>

<commit_message>
Added further functionalities for kli
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -9,22 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
     <sheet name="PremiumQuotePage" sheetId="23" r:id="rId2"/>
     <sheet name="ApplyDiscountPage" sheetId="24" r:id="rId3"/>
-    <sheet name="Resident Status Page" sheetId="26" r:id="rId4"/>
-    <sheet name="BenefitsPage" sheetId="27" r:id="rId5"/>
-    <sheet name="PayoutDetailsPage" sheetId="29" r:id="rId6"/>
-    <sheet name="PayPremiumPage" sheetId="28" r:id="rId7"/>
-    <sheet name="PersonalInformationPage" sheetId="25" r:id="rId8"/>
-    <sheet name="UploadDocsPage" sheetId="30" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="31" r:id="rId10"/>
+    <sheet name="AddOnPage" sheetId="26" r:id="rId4"/>
+    <sheet name="PayoutDetailsPage" sheetId="29" r:id="rId5"/>
+    <sheet name="PayPremiumPage" sheetId="28" r:id="rId6"/>
+    <sheet name="PersonalInformationPage" sheetId="25" r:id="rId7"/>
+    <sheet name="UploadDocsPage" sheetId="30" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="31" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="Abc">#REF!</definedName>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -66,39 +65,6 @@
     <t>Click</t>
   </si>
   <si>
-    <t>CustomerAccountName</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Actions</t>
-  </si>
-  <si>
-    <t>//input[@ng-model='CustomerSearchCriteria.AccountName']</t>
-  </si>
-  <si>
-    <t>//*[@id="div1"]/div/button</t>
-  </si>
-  <si>
-    <t>(//a[@class='vam-table-tdArrow'])[2]</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>Iframe</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>//*[@class='btn btn-blue']</t>
-  </si>
-  <si>
     <t>Locators</t>
   </si>
   <si>
@@ -168,9 +134,6 @@
     <t>//button[@class="btn-red btn-b done-btn"]</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>//input[@name="coverageAmount"]</t>
   </si>
   <si>
@@ -210,15 +173,6 @@
     <t>//button[@class="popup-main-btn p-0-override mt-35-override"]</t>
   </si>
   <si>
-    <t>Continue</t>
-  </si>
-  <si>
-    <t>//*[@id="benefitForm"]/section/div/section[1]/div[2]/div/div/ul/li[2]/div[1]/div[2]/div/button</t>
-  </si>
-  <si>
-    <t>LifePlus</t>
-  </si>
-  <si>
     <t>//button[@class="btn-red btn-b "]</t>
   </si>
   <si>
@@ -262,6 +216,87 @@
   </si>
   <si>
     <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>DiscountDone</t>
+  </si>
+  <si>
+    <t>AddOnContinue</t>
+  </si>
+  <si>
+    <t>ResidentContinue</t>
+  </si>
+  <si>
+    <t>ContinueToPayout</t>
+  </si>
+  <si>
+    <t>//input[@name="PanId"]</t>
+  </si>
+  <si>
+    <t>//input[@name="city"]</t>
+  </si>
+  <si>
+    <t>//input[@name="state"]</t>
+  </si>
+  <si>
+    <t>APJPV6335L</t>
+  </si>
+  <si>
+    <t>//input[@name="pin"]</t>
+  </si>
+  <si>
+    <t>StateDetails</t>
+  </si>
+  <si>
+    <t>CityDetails</t>
+  </si>
+  <si>
+    <t>PINcodeDetails</t>
+  </si>
+  <si>
+    <t>ContinueButton</t>
+  </si>
+  <si>
+    <t>PanDetails</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b"]</t>
+  </si>
+  <si>
+    <t>ContinueToPersonalDetails</t>
+  </si>
+  <si>
+    <t>//label[@class="agreement-checkbox"]</t>
+  </si>
+  <si>
+    <t>TermsCheckBox</t>
+  </si>
+  <si>
+    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[1]/div[2]/div/div[1]/div/ul/label[1]/li/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>//button[@class="ff-roboto-bold-override btn-red btn-b"]</t>
+  </si>
+  <si>
+    <t>ProceedToPay</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red"]</t>
+  </si>
+  <si>
+    <t>ContinueToPersonal</t>
+  </si>
+  <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>sleep=30000</t>
   </si>
 </sst>
 </file>
@@ -292,6 +327,7 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -315,21 +351,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Verdana"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -341,7 +379,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -397,17 +435,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -476,28 +503,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF505050"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color rgb="FF505050"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF505050"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF505050"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -519,9 +562,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -534,41 +574,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -589,6 +604,45 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1289,7 +1343,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,114 +1362,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="J2" s="29"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="G4" s="36">
+        <v>9999999999</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="32">
-        <v>9999999999</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="29"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -1427,8 +1481,8 @@
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -1440,7 +1494,7 @@
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -1453,7 +1507,7 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1461,25 +1515,25 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="12"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1492,7 +1546,7 @@
       <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1505,7 +1559,7 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1518,7 +1572,7 @@
       <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1539,26 +1593,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:J4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1582,63 +1622,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1664,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>3</v>
@@ -1689,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1739,7 @@
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
@@ -1735,22 +1775,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -1764,7 +1804,7 @@
       <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
-      <c r="U1" s="34"/>
+      <c r="U1" s="20"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -1777,26 +1817,26 @@
     </row>
     <row r="2" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1810,7 +1850,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="34"/>
+      <c r="U2" s="20"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
@@ -1823,7 +1863,7 @@
     </row>
     <row r="3" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1871,13 +1911,13 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="37"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="23"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
@@ -1906,13 +1946,13 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="36"/>
-      <c r="W5" s="38"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="24"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
@@ -1941,13 +1981,13 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="37"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="23"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
@@ -1976,13 +2016,13 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="38"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="24"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -2006,7 +2046,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="V8" s="39"/>
+      <c r="V8" s="25"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
@@ -2030,7 +2070,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="V9" s="39"/>
+      <c r="V9" s="25"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
@@ -2054,12 +2094,12 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="V10" s="39"/>
+      <c r="V10" s="25"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AC10" s="40"/>
+      <c r="AC10" s="26"/>
     </row>
     <row r="11" spans="1:34" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -2073,26 +2113,26 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="42"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="41"/>
-      <c r="AE11" s="41"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="U11" s="27"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="27"/>
+      <c r="X11" s="27"/>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AB11" s="27"/>
+      <c r="AC11" s="27"/>
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="27"/>
       <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
@@ -2109,26 +2149,26 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="27"/>
+      <c r="X12" s="27"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AB12" s="27"/>
+      <c r="AC12" s="27"/>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
     </row>
@@ -2148,13 +2188,13 @@
       <c r="M13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="37"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="23"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
@@ -2190,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,54 +2243,42 @@
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2259,96 +2287,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:AP10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>104</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2392,78 +2334,78 @@
     <col min="38" max="38" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>57</v>
+      <c r="C1" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="17"/>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="15"/>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="39"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -2486,102 +2428,463 @@
       <c r="AK2" s="5"/>
       <c r="AL2" s="5"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
+        <v>101</v>
+      </c>
+      <c r="B4" s="17">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="8"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="23"/>
-      <c r="AD4" s="23"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="23"/>
-      <c r="AH4" s="23"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="23"/>
-      <c r="AL4" s="24"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="W4" s="18"/>
+      <c r="X4" s="18"/>
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="19"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
       <c r="AL5" s="5"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
+      <c r="AK6" s="16"/>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="16"/>
+      <c r="AN6" s="16"/>
+      <c r="AO6" s="16"/>
+      <c r="AP6" s="15"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
+      <c r="AH7" s="5"/>
+      <c r="AI7" s="5"/>
+      <c r="AJ7" s="5"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="5"/>
+      <c r="AO7" s="5"/>
+      <c r="AP7" s="5"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="19"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
+      <c r="AP10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45">
+        <v>101</v>
+      </c>
+      <c r="B4" s="45">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="45">
+        <v>500072</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2591,173 +2894,120 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
-        <v>111</v>
-      </c>
-      <c r="B4" s="27">
-        <v>1</v>
-      </c>
-      <c r="C4" s="27">
-        <v>0</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2765,100 +3015,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>101</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>102</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>103</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
-        <v>106</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F3"/>
   <sheetViews>
@@ -2870,10 +3026,24 @@
   <sheetData>
     <row r="3" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
few changes to the kli data
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="249">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -646,9 +646,6 @@
     <t>104</t>
   </si>
   <si>
-    <t>IamCoveredUnderKotakGroupInsurance scheme through my employer</t>
-  </si>
-  <si>
     <t>SelectOrganization</t>
   </si>
   <si>
@@ -688,18 +685,12 @@
     <t>459 old street</t>
   </si>
   <si>
-    <t>screenshot()</t>
-  </si>
-  <si>
     <t>Screenshot</t>
   </si>
   <si>
     <t>Screenshot1</t>
   </si>
   <si>
-    <t>Screenshot()</t>
-  </si>
-  <si>
     <t>[data-value="txtBankIDBK-OTHER"]</t>
   </si>
   <si>
@@ -782,6 +773,33 @@
   </si>
   <si>
     <t>[class="ng-option ng-option-marked"]</t>
+  </si>
+  <si>
+    <t>sleep=5000</t>
+  </si>
+  <si>
+    <t>sleep=2000</t>
+  </si>
+  <si>
+    <t>IamCoveredUnderKotakGroupInsuranceSchemeThroughMyEmployer</t>
+  </si>
+  <si>
+    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[2]/label/div/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Mahindra &amp;')]</t>
+  </si>
+  <si>
+    <t>ClickOrganisation</t>
+  </si>
+  <si>
+    <t>[class="ng-arrow-wrapper"]</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[1]/label</t>
+  </si>
+  <si>
+    <t>sleep=40000</t>
   </si>
 </sst>
 </file>
@@ -876,7 +894,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -945,15 +963,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1090,15 +1099,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1106,6 +1110,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1805,7 +1814,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1813,8 +1822,8 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
@@ -1856,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L1" s="41"/>
     </row>
@@ -1871,8 +1880,8 @@
       <c r="D2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>16</v>
+      <c r="E2" s="54" t="s">
+        <v>247</v>
       </c>
       <c r="F2" s="28" t="s">
         <v>30</v>
@@ -1899,7 +1908,6 @@
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
@@ -1937,9 +1945,7 @@
       <c r="J4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="23" t="s">
-        <v>211</v>
-      </c>
+      <c r="K4" s="23"/>
       <c r="L4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1957,7 +1963,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>182</v>
@@ -2021,7 +2027,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>182</v>
@@ -2136,7 +2142,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,7 +2334,9 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2">
+        <v>10000</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="24"/>
       <c r="K3" s="3">
@@ -2494,8 +2502,64 @@
       <c r="B6" s="1">
         <v>10</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>12011985</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
@@ -2515,10 +2579,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,13 +2614,13 @@
         <v>161</v>
       </c>
       <c r="H1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K1" t="s">
         <v>112</v>
@@ -2577,19 +2641,19 @@
         <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H2" t="s">
         <v>235</v>
       </c>
-      <c r="H2" t="s">
-        <v>238</v>
-      </c>
       <c r="I2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="J2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2605,31 +2669,81 @@
       <c r="B4" s="3">
         <v>11</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="I4" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="48" t="s">
         <v>3</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>102</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>103</v>
+      </c>
+      <c r="B6" s="1">
+        <v>11</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6">
         <v>0</v>
       </c>
     </row>
@@ -2642,8 +2756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,7 +2806,7 @@
         <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2730,7 +2844,9 @@
         <v>5</v>
       </c>
       <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="C3" s="28">
+        <v>50000</v>
+      </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
@@ -2768,9 +2884,6 @@
       <c r="J4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>214</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
@@ -2865,50 +2978,53 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN14"/>
+  <dimension ref="A1:AO14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO14" sqref="AO3:EC14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="29.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" customWidth="1"/>
-    <col min="11" max="12" width="26.5703125" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" customWidth="1"/>
-    <col min="16" max="16" width="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.28515625" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" customWidth="1"/>
-    <col min="28" max="28" width="23.5703125" customWidth="1"/>
-    <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.28515625" customWidth="1"/>
-    <col min="32" max="34" width="22.85546875" customWidth="1"/>
-    <col min="35" max="36" width="15.5703125" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" customWidth="1"/>
+    <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="38.28515625" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" customWidth="1"/>
+    <col min="28" max="28" width="16.42578125" customWidth="1"/>
+    <col min="29" max="29" width="23.5703125" customWidth="1"/>
+    <col min="30" max="30" width="20" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.28515625" customWidth="1"/>
+    <col min="33" max="35" width="22.85546875" customWidth="1"/>
+    <col min="36" max="37" width="15.5703125" customWidth="1"/>
+    <col min="39" max="39" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2919,36 +3035,38 @@
         <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="10"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -2960,23 +3078,24 @@
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="10"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="32"/>
       <c r="AB1" s="10"/>
       <c r="AC1" s="10"/>
       <c r="AD1" s="10"/>
       <c r="AE1" s="10"/>
       <c r="AF1" s="10"/>
       <c r="AG1" s="10"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="5"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="10"/>
       <c r="AK1" s="5"/>
       <c r="AL1" s="5"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="5"/>
-    </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="5"/>
+    </row>
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2984,33 +3103,39 @@
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="F2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>201</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
@@ -3022,44 +3147,51 @@
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="32"/>
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
       <c r="AD2" s="10"/>
       <c r="AE2" s="10"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="5"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="10"/>
       <c r="AK2" s="5"/>
       <c r="AL2" s="5"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="5"/>
-    </row>
-    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="5"/>
+    </row>
+    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3">
+        <v>70000</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3000</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
+        <v>2000</v>
+      </c>
+      <c r="I3" s="3">
         <v>5000</v>
       </c>
-      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="10"/>
+      <c r="N3" s="3"/>
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
@@ -3071,9 +3203,9 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
-      <c r="AC3" s="10"/>
+      <c r="AC3" s="5"/>
       <c r="AD3" s="10"/>
-      <c r="AE3" s="5"/>
+      <c r="AE3" s="10"/>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
@@ -3083,8 +3215,9 @@
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
-    </row>
-    <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AO3" s="5"/>
+    </row>
+    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3096,25 +3229,25 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3">
         <v>1974551</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="10"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
@@ -3122,14 +3255,14 @@
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
-      <c r="V4" s="33"/>
+      <c r="V4" s="10"/>
       <c r="W4" s="33"/>
       <c r="X4" s="33"/>
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="10"/>
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="35"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
       <c r="AF4" s="10"/>
@@ -3137,12 +3270,13 @@
       <c r="AH4" s="10"/>
       <c r="AI4" s="10"/>
       <c r="AJ4" s="10"/>
-      <c r="AK4" s="5"/>
-      <c r="AL4" s="10"/>
+      <c r="AK4" s="10"/>
+      <c r="AL4" s="5"/>
       <c r="AM4" s="10"/>
-      <c r="AN4" s="5"/>
-    </row>
-    <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="5"/>
+    </row>
+    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -3154,19 +3288,19 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N5" s="10"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
@@ -3174,14 +3308,14 @@
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
-      <c r="V5" s="33"/>
+      <c r="V5" s="10"/>
       <c r="W5" s="33"/>
       <c r="X5" s="33"/>
       <c r="Y5" s="33"/>
       <c r="Z5" s="33"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="10"/>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="21"/>
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
@@ -3189,12 +3323,13 @@
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="5"/>
       <c r="AM5" s="10"/>
-      <c r="AN5" s="5"/>
-    </row>
-    <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="5"/>
+    </row>
+    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -3208,7 +3343,9 @@
       <c r="E6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>3</v>
@@ -3216,13 +3353,15 @@
       <c r="I6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="10"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
@@ -3230,14 +3369,14 @@
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
-      <c r="V6" s="33"/>
+      <c r="V6" s="10"/>
       <c r="W6" s="33"/>
       <c r="X6" s="33"/>
       <c r="Y6" s="33"/>
       <c r="Z6" s="33"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="10"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="35"/>
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
       <c r="AF6" s="10"/>
@@ -3245,12 +3384,13 @@
       <c r="AH6" s="10"/>
       <c r="AI6" s="10"/>
       <c r="AJ6" s="10"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="5"/>
       <c r="AM6" s="10"/>
-      <c r="AN6" s="5"/>
-    </row>
-    <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="5"/>
+    </row>
+    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>104</v>
       </c>
@@ -3262,23 +3402,23 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="10"/>
+      <c r="L7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
@@ -3286,14 +3426,14 @@
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
-      <c r="V7" s="33"/>
+      <c r="V7" s="10"/>
       <c r="W7" s="33"/>
       <c r="X7" s="33"/>
       <c r="Y7" s="33"/>
       <c r="Z7" s="33"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="10"/>
+      <c r="AA7" s="33"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="21"/>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
       <c r="AF7" s="10"/>
@@ -3301,12 +3441,13 @@
       <c r="AH7" s="10"/>
       <c r="AI7" s="10"/>
       <c r="AJ7" s="10"/>
-      <c r="AK7" s="5"/>
-      <c r="AL7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="5"/>
       <c r="AM7" s="10"/>
-      <c r="AN7" s="5"/>
-    </row>
-    <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="5"/>
+    </row>
+    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -3323,7 +3464,7 @@
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="5"/>
+      <c r="Q8" s="10"/>
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
@@ -3333,9 +3474,9 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
-      <c r="AA8" s="36"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="10"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="36"/>
+      <c r="AC8" s="5"/>
       <c r="AD8" s="10"/>
       <c r="AE8" s="10"/>
       <c r="AF8" s="10"/>
@@ -3343,12 +3484,13 @@
       <c r="AH8" s="10"/>
       <c r="AI8" s="10"/>
       <c r="AJ8" s="10"/>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="5"/>
       <c r="AM8" s="10"/>
-      <c r="AN8" s="5"/>
-    </row>
-    <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="5"/>
+    </row>
+    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -3365,7 +3507,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="10"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -3375,9 +3517,9 @@
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
       <c r="Z9" s="5"/>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="10"/>
+      <c r="AA9" s="5"/>
+      <c r="AB9" s="36"/>
+      <c r="AC9" s="5"/>
       <c r="AD9" s="10"/>
       <c r="AE9" s="10"/>
       <c r="AF9" s="10"/>
@@ -3385,12 +3527,13 @@
       <c r="AH9" s="10"/>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="10"/>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="10"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="5"/>
       <c r="AM9" s="10"/>
-      <c r="AN9" s="5"/>
-    </row>
-    <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN9" s="10"/>
+      <c r="AO9" s="5"/>
+    </row>
+    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -3407,7 +3550,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
-      <c r="Q10" s="5"/>
+      <c r="Q10" s="10"/>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
@@ -3417,22 +3560,23 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
       <c r="Z10" s="5"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="10"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="36"/>
+      <c r="AC10" s="5"/>
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="37"/>
-      <c r="AI10" s="5"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="37"/>
       <c r="AJ10" s="5"/>
       <c r="AK10" s="5"/>
       <c r="AL10" s="5"/>
       <c r="AM10" s="5"/>
       <c r="AN10" s="5"/>
-    </row>
-    <row r="11" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AO10" s="5"/>
+    </row>
+    <row r="11" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3449,7 +3593,7 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="38"/>
+      <c r="Q11" s="10"/>
       <c r="R11" s="38"/>
       <c r="S11" s="38"/>
       <c r="T11" s="38"/>
@@ -3459,8 +3603,8 @@
       <c r="X11" s="38"/>
       <c r="Y11" s="38"/>
       <c r="Z11" s="38"/>
-      <c r="AA11" s="39"/>
-      <c r="AB11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="39"/>
       <c r="AC11" s="38"/>
       <c r="AD11" s="38"/>
       <c r="AE11" s="38"/>
@@ -3469,12 +3613,13 @@
       <c r="AH11" s="38"/>
       <c r="AI11" s="38"/>
       <c r="AJ11" s="38"/>
-      <c r="AK11" s="10"/>
+      <c r="AK11" s="38"/>
       <c r="AL11" s="10"/>
       <c r="AM11" s="10"/>
-      <c r="AN11" s="5"/>
-    </row>
-    <row r="12" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="5"/>
+    </row>
+    <row r="12" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3491,7 +3636,7 @@
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="10"/>
-      <c r="Q12" s="38"/>
+      <c r="Q12" s="10"/>
       <c r="R12" s="38"/>
       <c r="S12" s="38"/>
       <c r="T12" s="38"/>
@@ -3501,8 +3646,8 @@
       <c r="X12" s="38"/>
       <c r="Y12" s="38"/>
       <c r="Z12" s="38"/>
-      <c r="AA12" s="39"/>
-      <c r="AB12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="39"/>
       <c r="AC12" s="38"/>
       <c r="AD12" s="38"/>
       <c r="AE12" s="38"/>
@@ -3511,12 +3656,13 @@
       <c r="AH12" s="38"/>
       <c r="AI12" s="38"/>
       <c r="AJ12" s="38"/>
-      <c r="AK12" s="5"/>
-      <c r="AL12" s="10"/>
+      <c r="AK12" s="38"/>
+      <c r="AL12" s="5"/>
       <c r="AM12" s="10"/>
-      <c r="AN12" s="5"/>
-    </row>
-    <row r="13" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="5"/>
+    </row>
+    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3535,17 +3681,17 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="5"/>
       <c r="U13" s="10"/>
-      <c r="V13" s="33"/>
+      <c r="V13" s="10"/>
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
       <c r="Y13" s="33"/>
       <c r="Z13" s="33"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="10"/>
+      <c r="AA13" s="33"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="35"/>
       <c r="AD13" s="10"/>
       <c r="AE13" s="10"/>
       <c r="AF13" s="10"/>
@@ -3553,12 +3699,13 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="10"/>
-      <c r="AK13" s="5"/>
-      <c r="AL13" s="10"/>
+      <c r="AK13" s="10"/>
+      <c r="AL13" s="5"/>
       <c r="AM13" s="10"/>
-      <c r="AN13" s="5"/>
-    </row>
-    <row r="14" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AN13" s="10"/>
+      <c r="AO13" s="5"/>
+    </row>
+    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -3575,7 +3722,7 @@
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="10"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
@@ -3599,10 +3746,11 @@
       <c r="AL14" s="5"/>
       <c r="AM14" s="5"/>
       <c r="AN14" s="5"/>
+      <c r="AO14" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="N5 P5 U5 AA4:AB7 AA13:AB13 P7 U7 N7"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="O5 Q5 V5 AB4:AC7 AB13:AC13 Q7 V7 O7"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3614,7 +3762,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,6 +3797,9 @@
         <v>5</v>
       </c>
       <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -3703,7 +3854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3765,40 +3916,40 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
+      <c r="AM1" s="49"/>
+      <c r="AN1" s="49"/>
+      <c r="AO1" s="49"/>
+      <c r="AP1" s="49"/>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3815,40 +3966,40 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -3861,40 +4012,40 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52"/>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="52"/>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="52"/>
-      <c r="AJ3" s="52"/>
-      <c r="AK3" s="52"/>
-      <c r="AL3" s="52"/>
-      <c r="AM3" s="52"/>
-      <c r="AN3" s="52"/>
-      <c r="AO3" s="52"/>
-      <c r="AP3" s="52"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
+      <c r="AA3" s="49"/>
+      <c r="AB3" s="49"/>
+      <c r="AC3" s="49"/>
+      <c r="AD3" s="49"/>
+      <c r="AE3" s="49"/>
+      <c r="AF3" s="49"/>
+      <c r="AG3" s="49"/>
+      <c r="AH3" s="49"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="49"/>
+      <c r="AK3" s="49"/>
+      <c r="AL3" s="49"/>
+      <c r="AM3" s="49"/>
+      <c r="AN3" s="49"/>
+      <c r="AO3" s="49"/>
+      <c r="AP3" s="49"/>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -3913,40 +4064,40 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="52"/>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="52"/>
-      <c r="Z4" s="52"/>
-      <c r="AA4" s="52"/>
-      <c r="AB4" s="52"/>
-      <c r="AC4" s="52"/>
-      <c r="AD4" s="52"/>
-      <c r="AE4" s="52"/>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52"/>
-      <c r="AH4" s="52"/>
-      <c r="AI4" s="52"/>
-      <c r="AJ4" s="52"/>
-      <c r="AK4" s="52"/>
-      <c r="AL4" s="52"/>
-      <c r="AM4" s="52"/>
-      <c r="AN4" s="52"/>
-      <c r="AO4" s="52"/>
-      <c r="AP4" s="52"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="49"/>
+      <c r="W4" s="49"/>
+      <c r="X4" s="49"/>
+      <c r="Y4" s="49"/>
+      <c r="Z4" s="49"/>
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49"/>
+      <c r="AC4" s="49"/>
+      <c r="AD4" s="49"/>
+      <c r="AE4" s="49"/>
+      <c r="AF4" s="49"/>
+      <c r="AG4" s="49"/>
+      <c r="AH4" s="49"/>
+      <c r="AI4" s="49"/>
+      <c r="AJ4" s="49"/>
+      <c r="AK4" s="49"/>
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -3965,40 +4116,40 @@
       <c r="F5" s="5"/>
       <c r="G5" s="10"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="52"/>
-      <c r="AA5" s="52"/>
-      <c r="AB5" s="52"/>
-      <c r="AC5" s="52"/>
-      <c r="AD5" s="52"/>
-      <c r="AE5" s="52"/>
-      <c r="AF5" s="52"/>
-      <c r="AG5" s="52"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="52"/>
-      <c r="AJ5" s="52"/>
-      <c r="AK5" s="52"/>
-      <c r="AL5" s="52"/>
-      <c r="AM5" s="52"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="52"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="49"/>
+      <c r="AK5" s="49"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="49"/>
+      <c r="AN5" s="49"/>
+      <c r="AO5" s="49"/>
+      <c r="AP5" s="49"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -4017,40 +4168,40 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="52"/>
-      <c r="Z6" s="52"/>
-      <c r="AA6" s="52"/>
-      <c r="AB6" s="52"/>
-      <c r="AC6" s="52"/>
-      <c r="AD6" s="52"/>
-      <c r="AE6" s="52"/>
-      <c r="AF6" s="52"/>
-      <c r="AG6" s="52"/>
-      <c r="AH6" s="52"/>
-      <c r="AI6" s="52"/>
-      <c r="AJ6" s="52"/>
-      <c r="AK6" s="52"/>
-      <c r="AL6" s="52"/>
-      <c r="AM6" s="52"/>
-      <c r="AN6" s="52"/>
-      <c r="AO6" s="52"/>
-      <c r="AP6" s="52"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+      <c r="W6" s="49"/>
+      <c r="X6" s="49"/>
+      <c r="Y6" s="49"/>
+      <c r="Z6" s="49"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="49"/>
+      <c r="AC6" s="49"/>
+      <c r="AD6" s="49"/>
+      <c r="AE6" s="49"/>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="49"/>
+      <c r="AH6" s="49"/>
+      <c r="AI6" s="49"/>
+      <c r="AJ6" s="49"/>
+      <c r="AK6" s="49"/>
+      <c r="AL6" s="49"/>
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="49"/>
+      <c r="AO6" s="49"/>
+      <c r="AP6" s="49"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -4069,160 +4220,160 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="V7" s="52"/>
-      <c r="W7" s="52"/>
-      <c r="X7" s="52"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="52"/>
-      <c r="AC7" s="52"/>
-      <c r="AD7" s="52"/>
-      <c r="AE7" s="52"/>
-      <c r="AF7" s="52"/>
-      <c r="AG7" s="52"/>
-      <c r="AH7" s="52"/>
-      <c r="AI7" s="52"/>
-      <c r="AJ7" s="52"/>
-      <c r="AK7" s="52"/>
-      <c r="AL7" s="52"/>
-      <c r="AM7" s="52"/>
-      <c r="AN7" s="52"/>
-      <c r="AO7" s="52"/>
-      <c r="AP7" s="52"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="49"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="49"/>
+      <c r="U7" s="49"/>
+      <c r="V7" s="49"/>
+      <c r="W7" s="49"/>
+      <c r="X7" s="49"/>
+      <c r="Y7" s="49"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="49"/>
+      <c r="AB7" s="49"/>
+      <c r="AC7" s="49"/>
+      <c r="AD7" s="49"/>
+      <c r="AE7" s="49"/>
+      <c r="AF7" s="49"/>
+      <c r="AG7" s="49"/>
+      <c r="AH7" s="49"/>
+      <c r="AI7" s="49"/>
+      <c r="AJ7" s="49"/>
+      <c r="AK7" s="49"/>
+      <c r="AL7" s="49"/>
+      <c r="AM7" s="49"/>
+      <c r="AN7" s="49"/>
+      <c r="AO7" s="49"/>
+      <c r="AP7" s="49"/>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="52"/>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="V8" s="52"/>
-      <c r="W8" s="52"/>
-      <c r="X8" s="52"/>
-      <c r="Y8" s="52"/>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="52"/>
-      <c r="AB8" s="52"/>
-      <c r="AC8" s="52"/>
-      <c r="AD8" s="52"/>
-      <c r="AE8" s="52"/>
-      <c r="AF8" s="52"/>
-      <c r="AG8" s="52"/>
-      <c r="AH8" s="52"/>
-      <c r="AI8" s="52"/>
-      <c r="AJ8" s="52"/>
-      <c r="AK8" s="52"/>
-      <c r="AL8" s="52"/>
-      <c r="AM8" s="52"/>
-      <c r="AN8" s="52"/>
-      <c r="AO8" s="52"/>
-      <c r="AP8" s="52"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Y8" s="49"/>
+      <c r="Z8" s="49"/>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
+      <c r="AK8" s="49"/>
+      <c r="AL8" s="49"/>
+      <c r="AM8" s="49"/>
+      <c r="AN8" s="49"/>
+      <c r="AO8" s="49"/>
+      <c r="AP8" s="49"/>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="52"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="V9" s="52"/>
-      <c r="W9" s="52"/>
-      <c r="X9" s="52"/>
-      <c r="Y9" s="52"/>
-      <c r="Z9" s="52"/>
-      <c r="AA9" s="52"/>
-      <c r="AB9" s="52"/>
-      <c r="AC9" s="52"/>
-      <c r="AD9" s="52"/>
-      <c r="AE9" s="52"/>
-      <c r="AF9" s="52"/>
-      <c r="AG9" s="52"/>
-      <c r="AH9" s="52"/>
-      <c r="AI9" s="52"/>
-      <c r="AJ9" s="52"/>
-      <c r="AK9" s="52"/>
-      <c r="AL9" s="52"/>
-      <c r="AM9" s="52"/>
-      <c r="AN9" s="52"/>
-      <c r="AO9" s="52"/>
-      <c r="AP9" s="52"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="49"/>
+      <c r="T9" s="49"/>
+      <c r="U9" s="49"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="49"/>
+      <c r="Y9" s="49"/>
+      <c r="Z9" s="49"/>
+      <c r="AA9" s="49"/>
+      <c r="AB9" s="49"/>
+      <c r="AC9" s="49"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="49"/>
+      <c r="AF9" s="49"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="49"/>
+      <c r="AJ9" s="49"/>
+      <c r="AK9" s="49"/>
+      <c r="AL9" s="49"/>
+      <c r="AM9" s="49"/>
+      <c r="AN9" s="49"/>
+      <c r="AO9" s="49"/>
+      <c r="AP9" s="49"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="52"/>
-      <c r="P10" s="52"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="52"/>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
-      <c r="W10" s="52"/>
-      <c r="X10" s="52"/>
-      <c r="Y10" s="52"/>
-      <c r="Z10" s="52"/>
-      <c r="AA10" s="52"/>
-      <c r="AB10" s="52"/>
-      <c r="AC10" s="52"/>
-      <c r="AD10" s="52"/>
-      <c r="AE10" s="52"/>
-      <c r="AF10" s="52"/>
-      <c r="AG10" s="52"/>
-      <c r="AH10" s="52"/>
-      <c r="AI10" s="52"/>
-      <c r="AJ10" s="52"/>
-      <c r="AK10" s="52"/>
-      <c r="AL10" s="52"/>
-      <c r="AM10" s="52"/>
-      <c r="AN10" s="52"/>
-      <c r="AO10" s="52"/>
-      <c r="AP10" s="52"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="49"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="49"/>
+      <c r="AM10" s="49"/>
+      <c r="AN10" s="49"/>
+      <c r="AO10" s="49"/>
+      <c r="AP10" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4235,7 +4386,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4431,8 +4582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4443,7 +4594,9 @@
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="9" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4516,12 +4669,14 @@
         <v>72</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="5"/>
@@ -4606,9 +4761,13 @@
       <c r="G6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="H6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
@@ -4651,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4666,11 +4825,10 @@
     <col min="7" max="7" width="16.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" style="5" customWidth="1"/>
+    <col min="10" max="11" width="15.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="5" customWidth="1"/>
     <col min="13" max="13" width="14" style="5" customWidth="1"/>
-    <col min="14" max="14" width="39" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.140625" style="5" customWidth="1"/>
     <col min="15" max="15" width="16.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -4700,26 +4858,26 @@
       <c r="H1" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="J1" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>230</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>231</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="I1" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="O1" t="s">
-        <v>229</v>
+      <c r="M1" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4745,26 +4903,26 @@
       <c r="H2" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="N2" t="s">
-        <v>226</v>
-      </c>
-      <c r="O2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -4778,6 +4936,17 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -4795,30 +4964,30 @@
       <c r="I4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="47" t="s">
-        <v>219</v>
+      <c r="J4" s="53" t="s">
+        <v>216</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="47" t="s">
-        <v>224</v>
+      <c r="L4" s="53" t="s">
+        <v>221</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>232</v>
+      <c r="N4" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="3">
         <v>102</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4839,22 +5008,69 @@
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="3">
         <v>103</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="3">
         <v>8</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="15">
         <v>104</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="3">
         <v>8</v>
       </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4867,7 +5083,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4950,7 +5166,7 @@
         <v>101</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -4983,7 +5199,7 @@
         <v>91</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L2" s="19" t="s">
         <v>94</v>
@@ -5162,10 +5378,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E6" s="3">
         <v>500001</v>
@@ -5210,6 +5426,9 @@
         <v>189</v>
       </c>
       <c r="S6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5221,10 +5440,10 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7" s="3">
         <v>500001</v>

</xml_diff>

<commit_message>
Fixed click intercepted wait issue. Increased implicit wait time
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5411859-28BF-4827-B030-74D8A50EE337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" firstSheet="9" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="223">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -62,376 +63,568 @@
     <t>Flow</t>
   </si>
   <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>TobaccoUserNo</t>
+  </si>
+  <si>
+    <t>TobaccoUserYes</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ViewQuote</t>
+  </si>
+  <si>
+    <t>Locators</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Male')]</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[2]/label</t>
+  </si>
+  <si>
+    <t>//*[@id="mat-input-0"]</t>
+  </si>
+  <si>
+    <t>//*[@id="full_name"]</t>
+  </si>
+  <si>
+    <t>//*[@id="phone"]</t>
+  </si>
+  <si>
+    <t>//*[@id="email"]</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[4]/div/div/button</t>
+  </si>
+  <si>
+    <t>ExplicitWait</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>Click</t>
   </si>
   <si>
-    <t>Locators</t>
-  </si>
-  <si>
-    <t>ExplicitWait</t>
-  </si>
-  <si>
-    <t>101</t>
+    <t>21/11/1987</t>
+  </si>
+  <si>
+    <t>Vijay Pawar</t>
+  </si>
+  <si>
+    <t>abc@abc.com</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>21/11/1995</t>
+  </si>
+  <si>
+    <t>Abc Xyz</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>CoverageAmount</t>
+  </si>
+  <si>
+    <t>AnnualIncome</t>
+  </si>
+  <si>
+    <t>AnnualIncomePopUp</t>
+  </si>
+  <si>
+    <t>AnnualIncomeDone</t>
+  </si>
+  <si>
+    <t>PGQualification</t>
+  </si>
+  <si>
+    <t>GradQualification</t>
+  </si>
+  <si>
+    <t>QualificationDone</t>
+  </si>
+  <si>
+    <t>GetKotakLifeDiscount</t>
+  </si>
+  <si>
+    <t>//input[@name="coverageAmount"]</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/section/div[3]/form/div[4]/div[2]/div</t>
+  </si>
+  <si>
+    <t>//input[@name='annual_income']</t>
+  </si>
+  <si>
+    <t>CSS = button[type='submit']</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[2]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>//*[@class="popup-main-btn"]</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Get Kotak Life Discount')]</t>
+  </si>
+  <si>
+    <t>10,00,000</t>
+  </si>
+  <si>
+    <t>im an existing kotak customer</t>
+  </si>
+  <si>
+    <t>IamCoveredUnderKotakGroupInsurance scheme through my employer</t>
+  </si>
+  <si>
+    <t>SelectOrganization</t>
+  </si>
+  <si>
+    <t>Policy no.</t>
+  </si>
+  <si>
+    <t>DiscountDone</t>
+  </si>
+  <si>
+    <t>PROCEEDTOCUSTOMIZE</t>
+  </si>
+  <si>
+    <t>YourResidentStatusIndian</t>
+  </si>
+  <si>
+    <t>YourResidentStatusNRI</t>
+  </si>
+  <si>
+    <t>PlanToVisit</t>
+  </si>
+  <si>
+    <t>ReturnDay</t>
+  </si>
+  <si>
+    <t>ResidentContinue</t>
+  </si>
+  <si>
+    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[1]/label/div/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>//input[@name="policyno"]</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b done-btn"]</t>
+  </si>
+  <si>
+    <t>//button[@class="main-cta"]</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Indian')]</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[2]/div/label[1]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>//input[@name="returnDate"]</t>
+  </si>
+  <si>
+    <t>//button[@class="popup-main-btn p-0-override mt-35-override"]</t>
+  </si>
+  <si>
+    <t>01022020</t>
+  </si>
+  <si>
+    <t>AddOnContinue</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b "]</t>
+  </si>
+  <si>
+    <t>ImmediatePayout</t>
+  </si>
+  <si>
+    <t>ContinueToPayout</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-payout-details/main/section/div[1]/section/div[2]/div/div/ul/label[1]/li/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>PanDetails</t>
+  </si>
+  <si>
+    <t>PINcodeDetails</t>
+  </si>
+  <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
+    <t>ContinueButton</t>
+  </si>
+  <si>
+    <t>//input[@name="PanId"]</t>
+  </si>
+  <si>
+    <t>//input[@name="pin"]</t>
+  </si>
+  <si>
+    <t>sleep=5000</t>
+  </si>
+  <si>
+    <t>APJPV6335L</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>ContinueToPersonalDetails</t>
+  </si>
+  <si>
+    <t>TermsCheckBox</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>ProceedToPay</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>ConfirmAndProceed</t>
+  </si>
+  <si>
+    <t>ContinueToPersonal</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b"]</t>
+  </si>
+  <si>
+    <t>//*[@id="premiumAgreementForm"]/section/div/section/div[2]/div/div/div/ul/li/div[1]/label</t>
+  </si>
+  <si>
+    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[1]/div[2]/div/div[1]/div/ul/label[1]/li/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[2]/div/button[2]</t>
+  </si>
+  <si>
+    <t>//input[@id="ContentPlaceHolder1_rbodisclaimer_0"]</t>
+  </si>
+  <si>
+    <t>//input[@id="ContentPlaceHolder1_btnPay"]</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red"]</t>
+  </si>
+  <si>
+    <t>input[type="checkbox"] + label:before</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>ExpiryDateMM</t>
+  </si>
+  <si>
+    <t>ExpiryDateYYYY</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CardHolderName</t>
+  </si>
+  <si>
+    <t>MakePayment</t>
+  </si>
+  <si>
+    <t>//*[@id="cnumber"]</t>
+  </si>
+  <si>
+    <t>//*[@id="expmon"]</t>
+  </si>
+  <si>
+    <t>//*[@id="expyr"]</t>
+  </si>
+  <si>
+    <t>//*[@id="cvv2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="cname2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="proceedForm"]</t>
+  </si>
+  <si>
+    <t>5123-4567-8901-2346</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Abc xyz</t>
+  </si>
+  <si>
+    <t>Addressline1</t>
+  </si>
+  <si>
+    <t>AdressLine2</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>LandMark</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>COntinue</t>
+  </si>
+  <si>
+    <t>YourOccupation</t>
+  </si>
+  <si>
+    <t>YourMaritalStatus</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>YourWeight</t>
+  </si>
+  <si>
+    <t>YourHeightInFeet</t>
+  </si>
+  <si>
+    <t>SelectHeightInFeet</t>
+  </si>
+  <si>
+    <t>YourHeightInInches</t>
+  </si>
+  <si>
+    <t>SelectHeightInInches</t>
+  </si>
+  <si>
+    <t>YourFatherName</t>
+  </si>
+  <si>
+    <t>YourMotherName</t>
+  </si>
+  <si>
+    <t>CONtinue</t>
+  </si>
+  <si>
+    <t>//input[@name="addressline1"]</t>
+  </si>
+  <si>
+    <t>//input[@name="addressline2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/input</t>
+  </si>
+  <si>
+    <t>//input[@name="landmark"]</t>
+  </si>
+  <si>
+    <t>//input[@class="ng-untouched ng-pristine ng-valid"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[1]/div[2]/div/div/label[1]/div/span[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/div/ng-select/div</t>
+  </si>
+  <si>
+    <t>//*[@class="ng-option ng-option-marked ng-star-inserted"]</t>
+  </si>
+  <si>
+    <t>//input[@name="weight"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[1]/ng-select/div</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[1]/ng-select/ng-dropdown-panel/div/div[2]/div[4]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[2]/ng-select/div</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[2]/ng-select/ng-dropdown-panel/div/div[2]/div[1]</t>
+  </si>
+  <si>
+    <t>//input[@name="fatherorspouseName"]</t>
+  </si>
+  <si>
+    <t>//input[@name="motherName"]</t>
+  </si>
+  <si>
+    <t>sleep=30000</t>
+  </si>
+  <si>
+    <t>123 new street</t>
+  </si>
+  <si>
+    <t>456 old street</t>
+  </si>
+  <si>
+    <t>mantri cosmos</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>suddgf sdgs</t>
+  </si>
+  <si>
+    <t>ghmfg gsgg</t>
+  </si>
+  <si>
+    <t>124 new street</t>
+  </si>
+  <si>
+    <t>457 old street</t>
+  </si>
+  <si>
+    <t>suddgf sdgk</t>
+  </si>
+  <si>
+    <t>ghmfg gsgl</t>
+  </si>
+  <si>
+    <t>125 new street</t>
+  </si>
+  <si>
+    <t>458 old street</t>
+  </si>
+  <si>
+    <t>126 new street</t>
+  </si>
+  <si>
+    <t>459 old street</t>
   </si>
   <si>
     <t>C:\Users\praneethm\Downloads\01T021344_Benefitillustration.pdf</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>NomineeGender</t>
+  </si>
+  <si>
+    <t>NomineeName</t>
+  </si>
+  <si>
+    <t>NomineeDOB</t>
+  </si>
+  <si>
+    <t>RelationshipWithAssured</t>
+  </si>
+  <si>
+    <t>SelectRelation</t>
+  </si>
+  <si>
+    <t>CONTinue</t>
+  </si>
+  <si>
+    <t>How Regularly Do you smoke?</t>
+  </si>
+  <si>
+    <t>Since When you have been smoking</t>
+  </si>
+  <si>
+    <t>CONTInue</t>
+  </si>
+  <si>
+    <t>CONTINue</t>
+  </si>
+  <si>
+    <t>CONTINUe</t>
+  </si>
+  <si>
+    <t>CONTINUE1</t>
+  </si>
+  <si>
+    <t>TaxResidentStatus</t>
+  </si>
+  <si>
+    <t>ResidentStatusDone</t>
   </si>
   <si>
     <t>TobaccoUser</t>
   </si>
   <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>MobileNumber</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>ViewQuote</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Male')]</t>
-  </si>
-  <si>
-    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[2]/label</t>
-  </si>
-  <si>
-    <t>//*[@id="full_name"]</t>
-  </si>
-  <si>
-    <t>//*[@id="phone"]</t>
-  </si>
-  <si>
-    <t>//*[@id="getQuoteForm"]/section[4]/div/div/button</t>
-  </si>
-  <si>
-    <t>21/11/1987</t>
-  </si>
-  <si>
-    <t>Vijay Pawar</t>
-  </si>
-  <si>
-    <t>CoverageAmount</t>
-  </si>
-  <si>
-    <t>im an existing kotak customer</t>
-  </si>
-  <si>
-    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[1]/label/div/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b done-btn"]</t>
-  </si>
-  <si>
-    <t>//input[@name="coverageAmount"]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/section/div[3]/form/div[4]/div[2]/div</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Get Kotak Life Discount')]</t>
-  </si>
-  <si>
-    <t>GetKotakLifeDiscount</t>
-  </si>
-  <si>
-    <t>//*[@id="mat-input-0"]</t>
-  </si>
-  <si>
-    <t>//*[@id="email"]</t>
-  </si>
-  <si>
-    <t>abc@abc.com</t>
-  </si>
-  <si>
-    <t>Policy no.</t>
-  </si>
-  <si>
-    <t>//input[@name="policyno"]</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Indian')]</t>
-  </si>
-  <si>
-    <t>//button[@class="popup-main-btn p-0-override mt-35-override"]</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b "]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-payout-details/main/section/div[1]/section/div[2]/div/div/ul/label[1]/li/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>ImmediatePayout</t>
-  </si>
-  <si>
-    <t>//button[@class="main-cta"]</t>
-  </si>
-  <si>
-    <t>PROCEEDTOCUSTOMIZE</t>
-  </si>
-  <si>
-    <t>AnnualIncomePopUp</t>
-  </si>
-  <si>
-    <t>//input[@name='annual_income']</t>
-  </si>
-  <si>
-    <t>AnnualIncome</t>
-  </si>
-  <si>
-    <t>10,00,000</t>
-  </si>
-  <si>
-    <t>//*[@class="popup-main-btn"]</t>
-  </si>
-  <si>
-    <t>PGQualification</t>
-  </si>
-  <si>
-    <t>CSS = button[type='submit']</t>
-  </si>
-  <si>
-    <t>AnnualIncomeDone</t>
-  </si>
-  <si>
-    <t>QualificationDone</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>DiscountDone</t>
-  </si>
-  <si>
-    <t>AddOnContinue</t>
-  </si>
-  <si>
-    <t>ResidentContinue</t>
-  </si>
-  <si>
-    <t>ContinueToPayout</t>
-  </si>
-  <si>
-    <t>//input[@name="PanId"]</t>
-  </si>
-  <si>
-    <t>APJPV6335L</t>
-  </si>
-  <si>
-    <t>//input[@name="pin"]</t>
-  </si>
-  <si>
-    <t>PINcodeDetails</t>
-  </si>
-  <si>
-    <t>ContinueButton</t>
-  </si>
-  <si>
-    <t>PanDetails</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b"]</t>
-  </si>
-  <si>
-    <t>ContinueToPersonalDetails</t>
-  </si>
-  <si>
-    <t>TermsCheckBox</t>
-  </si>
-  <si>
-    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[1]/div[2]/div/div[1]/div/ul/label[1]/li/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>PaymentMode</t>
-  </si>
-  <si>
-    <t>ProceedToPay</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red"]</t>
-  </si>
-  <si>
-    <t>ContinueToPersonal</t>
-  </si>
-  <si>
-    <t>ControlKeys</t>
-  </si>
-  <si>
-    <t>Tab</t>
-  </si>
-  <si>
-    <t>sleep=30000</t>
-  </si>
-  <si>
-    <t>//input[@name="addressline1"]</t>
-  </si>
-  <si>
-    <t>Addressline1</t>
-  </si>
-  <si>
-    <t>//input[@name="addressline2"]</t>
-  </si>
-  <si>
-    <t>AdressLine2</t>
-  </si>
-  <si>
-    <t>PinCode</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/input</t>
-  </si>
-  <si>
-    <t>LandMark</t>
-  </si>
-  <si>
-    <t>//input[@name="landmark"]</t>
-  </si>
-  <si>
-    <t>//input[@class="ng-untouched ng-pristine ng-valid"]</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>COntinue</t>
-  </si>
-  <si>
-    <t>input[type="checkbox"] + label:before</t>
-  </si>
-  <si>
-    <t>123 new street</t>
-  </si>
-  <si>
-    <t>456 old street</t>
-  </si>
-  <si>
-    <t>mantri cosmos</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>YourOccupation</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[1]/div[2]/div/div/label[1]/div/span[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/div/ng-select/div</t>
-  </si>
-  <si>
-    <t>YourMaritalStatus</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>//input[@name="weight"]</t>
-  </si>
-  <si>
-    <t>YourWeight</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[1]/ng-select/div</t>
-  </si>
-  <si>
-    <t>//input[@name="fatherorspouseName"]</t>
-  </si>
-  <si>
-    <t>YourFatherName</t>
-  </si>
-  <si>
-    <t>//input[@name="motherName"]</t>
-  </si>
-  <si>
-    <t>YourMotherName</t>
-  </si>
-  <si>
-    <t>CONtinue</t>
-  </si>
-  <si>
-    <t>SelectHeightInFeet</t>
-  </si>
-  <si>
-    <t>SelectHeightInInches</t>
-  </si>
-  <si>
-    <t>YourHeightInFeet</t>
-  </si>
-  <si>
-    <t>YourHeightInInches</t>
-  </si>
-  <si>
-    <t>suddgf sdgs</t>
-  </si>
-  <si>
-    <t>ghmfg gsgg</t>
+    <t>AadharDetails</t>
+  </si>
+  <si>
+    <t>IAgree1</t>
+  </si>
+  <si>
+    <t>InsuredOrProposer</t>
+  </si>
+  <si>
+    <t>IAgree2</t>
+  </si>
+  <si>
+    <t>ProposalForm</t>
+  </si>
+  <si>
+    <t>ThirdPartyPayment</t>
+  </si>
+  <si>
+    <t>IAgree3</t>
+  </si>
+  <si>
+    <t>Continue2</t>
   </si>
   <si>
     <t>//*[@id="nomineeForm"]/section[1]/div[2]/div[1]/div[1]/div/div/label[2]/div/span[1]</t>
   </si>
   <si>
-    <t>NomineeGender</t>
-  </si>
-  <si>
     <t>//input[@class="form-control ng-untouched ng-pristine ng-invalid"]</t>
   </si>
   <si>
-    <t>//*[@id="premiumAgreementForm"]/section/div/section/div[2]/div/div/div/ul/li/div[1]/label</t>
-  </si>
-  <si>
-    <t>Window</t>
-  </si>
-  <si>
-    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[2]/div/button[2]</t>
-  </si>
-  <si>
-    <t>//*[@class="ng-option ng-option-marked ng-star-inserted"]</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[2]/ng-select/div</t>
-  </si>
-  <si>
-    <t>NomineeName</t>
-  </si>
-  <si>
-    <t>NomineeDOB</t>
-  </si>
-  <si>
     <t>//input[@class="form-control input-date ng-untouched ng-pristine ng-invalid"]</t>
   </si>
   <si>
     <t>//*[@bindlabel="name"]</t>
   </si>
   <si>
-    <t>RelationshipWithAssured</t>
-  </si>
-  <si>
     <t>//*[@class="ng-option ng-star-inserted ng-option-marked"]</t>
   </si>
   <si>
-    <t>SelectRelation</t>
-  </si>
-  <si>
-    <t>CONTinue</t>
-  </si>
-  <si>
-    <t>CONTInue</t>
-  </si>
-  <si>
-    <t>CONTINue</t>
+    <t>//*[contains(text(),'Once a week')]</t>
+  </si>
+  <si>
+    <t>//*[@class="ng-select-container ng-has-value"]</t>
   </si>
   <si>
     <t>//*[@id="highriskForm"]/main/section/div/section/div/button[2]</t>
@@ -440,302 +633,107 @@
     <t>//*[@id="questionsForm"]/main/section/div/section/div/button[2]</t>
   </si>
   <si>
-    <t>CONTINUe</t>
-  </si>
-  <si>
     <t>//button[@class="popup-main-btn"]</t>
   </si>
   <si>
-    <t>CONTINUE1</t>
-  </si>
-  <si>
-    <t>TaxResidentStatus</t>
-  </si>
-  <si>
     <t>//*[@id="discountform"]/section/div/section[1]/div/div/div[1]/div/ul/li[1]/label/div/div[1]/div/span</t>
   </si>
   <si>
-    <t>ResidentStatusDone</t>
-  </si>
-  <si>
     <t>//*[@for="tandc"]</t>
   </si>
   <si>
     <t>//*[@for="tand8"]</t>
   </si>
   <si>
-    <t>AadharDetails</t>
-  </si>
-  <si>
-    <t>InsuredOrProposer</t>
-  </si>
-  <si>
-    <t>ProposalForm</t>
-  </si>
-  <si>
-    <t>ThirdPartyPayment</t>
-  </si>
-  <si>
-    <t>Continue2</t>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[3]/div[2]/div[2]/div[2]/button</t>
   </si>
   <si>
     <t>//*[@for="tand1"]</t>
   </si>
   <si>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[1]/div[2]/div[2]/div[2]/button</t>
+  </si>
+  <si>
     <t>//*[@for="tand3"]</t>
   </si>
   <si>
     <t>//*[@for="tand5"]</t>
   </si>
   <si>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[2]/div[2]/div[2]/div[2]/button</t>
+  </si>
+  <si>
     <t>//button[@class="ff-roboto-bold-override btn-red btn-b lts-30-override"]</t>
   </si>
   <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[3]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree1</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[1]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree2</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[2]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree3</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[1]/ng-select/ng-dropdown-panel/div/div[2]/div[4]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[2]/ng-select/ng-dropdown-panel/div/div[2]/div[1]</t>
-  </si>
-  <si>
-    <t>sleep=10000</t>
+    <t>Browse1</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>ControlKeys1</t>
+  </si>
+  <si>
+    <t>Browse2</t>
+  </si>
+  <si>
+    <t>Alert2</t>
+  </si>
+  <si>
+    <t>ControlKeys2</t>
+  </si>
+  <si>
+    <t>Browse3</t>
+  </si>
+  <si>
+    <t>Alert3</t>
+  </si>
+  <si>
+    <t>ControlKeys3</t>
+  </si>
+  <si>
+    <t>Browse4</t>
+  </si>
+  <si>
+    <t>Alert4</t>
+  </si>
+  <si>
+    <t>ControlKeys4</t>
+  </si>
+  <si>
+    <t>Browse5</t>
+  </si>
+  <si>
+    <t>Alert5</t>
+  </si>
+  <si>
+    <t>ControlKeys5</t>
   </si>
   <si>
     <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[1]/div[2]/button</t>
   </si>
   <si>
-    <t>Browse1</t>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[2]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[3]/div[2]/button</t>
   </si>
   <si>
     <t>C:\Users\praneethm\Downloads\01T021466_Benefitillustration.pdf</t>
   </si>
   <si>
-    <t>Alert</t>
-  </si>
-  <si>
     <t>Enter</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>Browse2</t>
-  </si>
-  <si>
-    <t>Alert2</t>
-  </si>
-  <si>
-    <t>ControlKeys1</t>
-  </si>
-  <si>
-    <t>ControlKeys2</t>
-  </si>
-  <si>
-    <t>Browse3</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[3]/div[2]/button</t>
-  </si>
-  <si>
-    <t>Alert3</t>
-  </si>
-  <si>
-    <t>ControlKeys3</t>
-  </si>
-  <si>
-    <t>Browse4</t>
-  </si>
-  <si>
-    <t>Alert4</t>
-  </si>
-  <si>
-    <t>ControlKeys4</t>
-  </si>
-  <si>
-    <t>Browse5</t>
-  </si>
-  <si>
-    <t>Alert5</t>
-  </si>
-  <si>
-    <t>ControlKeys5</t>
-  </si>
-  <si>
-    <t>sleep=5000</t>
-  </si>
-  <si>
-    <t>//input[@id="ContentPlaceHolder1_rbodisclaimer_0"]</t>
-  </si>
-  <si>
-    <t>Confirmation</t>
-  </si>
-  <si>
-    <t>//input[@id="ContentPlaceHolder1_btnPay"]</t>
-  </si>
-  <si>
-    <t>ConfirmAndProceed</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>ExpiryDateMM</t>
-  </si>
-  <si>
-    <t>ExpiryDateYYYY</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>CardHolderName</t>
-  </si>
-  <si>
-    <t>MakePayment</t>
-  </si>
-  <si>
-    <t>5123-4567-8901-2346</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>Abc xyz</t>
-  </si>
-  <si>
-    <t>//*[@id="cnumber"]</t>
-  </si>
-  <si>
-    <t>//*[@id="expmon"]</t>
-  </si>
-  <si>
-    <t>//*[@id="expyr"]</t>
-  </si>
-  <si>
-    <t>//*[@id="cvv2"]</t>
-  </si>
-  <si>
-    <t>//*[@id="cname2"]</t>
-  </si>
-  <si>
-    <t>//*[@id="proceedForm"]</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>Abc Xyz</t>
-  </si>
-  <si>
-    <t>TobaccoUserNo</t>
-  </si>
-  <si>
-    <t>TobaccoUserYes</t>
-  </si>
-  <si>
-    <t>GradQualification</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[2]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>124 new street</t>
-  </si>
-  <si>
-    <t>457 old street</t>
-  </si>
-  <si>
-    <t>ghmfg gsgl</t>
-  </si>
-  <si>
-    <t>suddgf sdgk</t>
-  </si>
-  <si>
-    <t>How Regularly Do you smoke?</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Once a week')]</t>
-  </si>
-  <si>
-    <t>Since When you have been smoking</t>
-  </si>
-  <si>
-    <t>//*[@class="ng-select-container ng-has-value"]</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>IamCoveredUnderKotakGroupInsurance scheme through my employer</t>
-  </si>
-  <si>
-    <t>SelectOrganization</t>
-  </si>
-  <si>
-    <t>YourResidentStatusIndian</t>
-  </si>
-  <si>
-    <t>YourResidentStatusNRI</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[2]/div/label[1]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>PlanToVisit</t>
-  </si>
-  <si>
-    <t>//input[@name="returnDate"]</t>
-  </si>
-  <si>
-    <t>ReturnDay</t>
-  </si>
-  <si>
-    <t>01022020</t>
-  </si>
-  <si>
-    <t>21/11/1995</t>
-  </si>
-  <si>
-    <t>125 new street</t>
-  </si>
-  <si>
-    <t>126 new street</t>
-  </si>
-  <si>
-    <t>458 old street</t>
-  </si>
-  <si>
-    <t>459 old street</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,7 +1120,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1787,14 +1785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1810,7 +1808,7 @@
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -1818,67 +1816,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="35" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K1" s="30"/>
       <c r="L1" s="49"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="I2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="35" t="s">
+      <c r="J2" s="35" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>19</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="35" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -1892,135 +1890,135 @@
       <c r="K3" s="30"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="51" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="34" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="33">
         <v>9999999999</v>
       </c>
       <c r="I4" s="35" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K4" s="30"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="51" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="H5" s="33">
         <v>9999999999</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="52" t="s">
-        <v>208</v>
+        <v>28</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="36" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H6" s="29">
         <v>9999999999</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="53" t="s">
-        <v>209</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
       <c r="H7" s="33">
         <v>9999999999</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="48"/>
       <c r="B8" s="17"/>
       <c r="C8" s="5"/>
@@ -2034,7 +2032,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="48"/>
       <c r="B9" s="17"/>
       <c r="C9" s="5"/>
@@ -2048,7 +2046,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="44"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="48"/>
       <c r="B10" s="17"/>
       <c r="C10" s="5"/>
@@ -2062,7 +2060,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="48"/>
       <c r="B11" s="17"/>
       <c r="C11" s="5"/>
@@ -2076,7 +2074,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="48"/>
       <c r="B12" s="17"/>
       <c r="C12" s="5"/>
@@ -2090,7 +2088,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="48"/>
       <c r="B13" s="17"/>
       <c r="C13" s="5"/>
@@ -2104,7 +2102,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="E16" s="30"/>
     </row>
   </sheetData>
@@ -2114,14 +2112,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
@@ -2142,7 +2140,7 @@
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2150,157 +2148,157 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>125</v>
+        <v>169</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>146</v>
+        <v>176</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>150</v>
+        <v>181</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>118</v>
+        <v>185</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>121</v>
+        <v>187</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>134</v>
+        <v>194</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>135</v>
+        <v>195</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>141</v>
+        <v>197</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2" t="s">
-        <v>143</v>
+        <v>200</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -2328,7 +2326,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -2336,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -2345,60 +2343,60 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="31"/>
       <c r="K4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="W4" s="3">
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -2406,70 +2404,70 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
         <v>12011987</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="W5" s="2">
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -2479,7 +2477,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" s="21">
         <v>104</v>
       </c>
@@ -2496,19 +2494,19 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2516,73 +2514,73 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>205</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="H1" t="s">
-        <v>163</v>
+        <v>208</v>
       </c>
       <c r="I1" t="s">
-        <v>164</v>
+        <v>209</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="L1" t="s">
-        <v>168</v>
+        <v>212</v>
       </c>
       <c r="M1" t="s">
-        <v>169</v>
+        <v>213</v>
       </c>
       <c r="N1" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="O1" t="s">
-        <v>171</v>
+        <v>215</v>
       </c>
       <c r="P1" t="s">
-        <v>172</v>
+        <v>216</v>
       </c>
       <c r="Q1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>218</v>
       </c>
       <c r="F2" t="s">
-        <v>159</v>
+        <v>219</v>
       </c>
       <c r="I2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -2590,13 +2588,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2605,28 +2603,28 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -2639,7 +2637,7 @@
     <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
@@ -2647,63 +2645,63 @@
         <v>1</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>198</v>
+        <v>35</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="35" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E2" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>199</v>
-      </c>
       <c r="I2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="35" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1">
       <c r="A3" s="35" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -2715,7 +2713,7 @@
       <c r="I3" s="35"/>
       <c r="J3" s="35"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1">
       <c r="A4" s="35">
         <v>101</v>
       </c>
@@ -2726,26 +2724,26 @@
         <v>25000000</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H4" s="35"/>
       <c r="I4" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="35">
         <v>102</v>
       </c>
@@ -2756,24 +2754,24 @@
         <v>25000000</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5" s="33">
         <v>200000</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G5" s="35"/>
       <c r="H5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I5" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J5" s="35"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="35">
         <v>103</v>
       </c>
@@ -2784,26 +2782,26 @@
         <v>25000000</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6" s="35">
         <v>1000000</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="38">
         <v>104</v>
       </c>
@@ -2814,20 +2812,20 @@
         <v>25000000</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E7" s="33">
         <v>200000</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G7" s="35"/>
       <c r="H7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J7" s="35"/>
     </row>
@@ -2837,14 +2835,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AN14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -2881,7 +2879,7 @@
     <col min="39" max="39" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2889,37 +2887,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>210</v>
+        <v>48</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>211</v>
+        <v>49</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>212</v>
+        <v>53</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>213</v>
+        <v>54</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>215</v>
+        <v>55</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>217</v>
+        <v>56</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
@@ -2949,39 +2947,39 @@
       <c r="AM1" s="17"/>
       <c r="AN1" s="5"/>
     </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>214</v>
+        <v>63</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>216</v>
+        <v>64</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
@@ -3011,9 +3009,9 @@
       <c r="AM2" s="17"/>
       <c r="AN2" s="5"/>
     </row>
-    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" s="2" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3055,7 +3053,7 @@
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
     </row>
-    <row r="4" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" s="2" customFormat="1">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3063,7 +3061,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -3071,19 +3069,19 @@
         <v>1974551</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
@@ -3113,7 +3111,7 @@
       <c r="AM4" s="17"/>
       <c r="AN4" s="5"/>
     </row>
-    <row r="5" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" s="2" customFormat="1">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -3126,16 +3124,16 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
@@ -3165,7 +3163,7 @@
       <c r="AM5" s="17"/>
       <c r="AN5" s="5"/>
     </row>
-    <row r="6" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="2" customFormat="1">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -3174,24 +3172,24 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
@@ -3221,7 +3219,7 @@
       <c r="AM6" s="17"/>
       <c r="AN6" s="5"/>
     </row>
-    <row r="7" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" s="2" customFormat="1">
       <c r="A7" s="3">
         <v>104</v>
       </c>
@@ -3234,20 +3232,20 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>218</v>
+        <v>66</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
@@ -3277,7 +3275,7 @@
       <c r="AM7" s="17"/>
       <c r="AN7" s="5"/>
     </row>
-    <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" s="2" customFormat="1">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -3319,7 +3317,7 @@
       <c r="AM8" s="17"/>
       <c r="AN8" s="5"/>
     </row>
-    <row r="9" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" s="2" customFormat="1">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
@@ -3361,7 +3359,7 @@
       <c r="AM9" s="17"/>
       <c r="AN9" s="5"/>
     </row>
-    <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" s="2" customFormat="1">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
@@ -3403,7 +3401,7 @@
       <c r="AM10" s="5"/>
       <c r="AN10" s="5"/>
     </row>
-    <row r="11" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -3445,7 +3443,7 @@
       <c r="AM11" s="17"/>
       <c r="AN11" s="5"/>
     </row>
-    <row r="12" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -3487,7 +3485,7 @@
       <c r="AM12" s="17"/>
       <c r="AN12" s="5"/>
     </row>
-    <row r="13" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" s="2" customFormat="1">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -3529,7 +3527,7 @@
       <c r="AM13" s="17"/>
       <c r="AN13" s="5"/>
     </row>
-    <row r="14" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" s="2" customFormat="1">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -3573,7 +3571,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="N5 P5 U5 AA4:AB7 AA13:AB13 P7 U7 N7"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="N5 P5 U5 AA4:AB7 AA13:AB13 P7 U7 N7" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3581,21 +3579,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3603,25 +3601,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3629,10 +3627,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -3640,10 +3638,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -3651,10 +3649,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="21">
         <v>104</v>
       </c>
@@ -3662,7 +3660,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3671,14 +3669,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AP10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
@@ -3719,7 +3717,7 @@
     <col min="38" max="38" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3727,10 +3725,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3767,16 +3765,16 @@
       <c r="AK1" s="8"/>
       <c r="AL1" s="7"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -3813,9 +3811,9 @@
       <c r="AK2" s="4"/>
       <c r="AL2" s="4"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3833,7 +3831,7 @@
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3841,10 +3839,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -3881,7 +3879,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -3889,10 +3887,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3929,7 +3927,7 @@
       <c r="AK5" s="6"/>
       <c r="AL5" s="4"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -3937,10 +3935,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3981,7 +3979,7 @@
       <c r="AO6" s="8"/>
       <c r="AP6" s="7"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42">
       <c r="A7" s="3">
         <v>104</v>
       </c>
@@ -3989,10 +3987,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4033,7 +4031,7 @@
       <c r="AO7" s="4"/>
       <c r="AP7" s="4"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42">
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -4047,7 +4045,7 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42">
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="5"/>
@@ -4087,7 +4085,7 @@
       <c r="AO9" s="9"/>
       <c r="AP9" s="10"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42">
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="5"/>
@@ -4134,14 +4132,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
@@ -4151,7 +4149,7 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4159,56 +4157,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.5" customHeight="1">
       <c r="A2" s="19" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="19" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="19" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="20" t="s">
-        <v>174</v>
+        <v>78</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" customHeight="1">
       <c r="A4" s="20">
         <v>101</v>
       </c>
@@ -4216,22 +4214,22 @@
         <v>6</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D4" s="20">
         <v>500072</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -4239,22 +4237,22 @@
         <v>6</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D5" s="20">
         <v>500072</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -4262,22 +4260,22 @@
         <v>6</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D6" s="20">
         <v>500072</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>104</v>
       </c>
@@ -4285,40 +4283,40 @@
         <v>6</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D7" s="20">
         <v>500072</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -4331,14 +4329,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -4350,7 +4348,7 @@
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4358,69 +4356,65 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>176</v>
+        <v>86</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>178</v>
+        <v>87</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>175</v>
+        <v>93</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>177</v>
+        <v>94</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>153</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -4431,7 +4425,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4439,29 +4433,29 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="17">
         <v>102</v>
       </c>
@@ -4469,25 +4463,25 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="17">
         <v>103</v>
       </c>
@@ -4495,25 +4489,25 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="21">
         <v>104</v>
       </c>
@@ -4521,27 +4515,27 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="D13" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -4551,14 +4545,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="5"/>
@@ -4571,7 +4565,7 @@
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4579,53 +4573,53 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>179</v>
+        <v>97</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>182</v>
+        <v>100</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>183</v>
+        <v>101</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>184</v>
+        <v>102</v>
       </c>
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>188</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>190</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>191</v>
+        <v>106</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>192</v>
+        <v>107</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -4635,7 +4629,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4643,10 +4637,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>185</v>
+        <v>109</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>186</v>
+        <v>110</v>
       </c>
       <c r="E4" s="3">
         <v>2020</v>
@@ -4655,15 +4649,15 @@
         <v>123</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>187</v>
+        <v>111</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="5">
         <v>102</v>
       </c>
@@ -4671,7 +4665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="5">
         <v>103</v>
       </c>
@@ -4679,7 +4673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="47">
         <v>104</v>
       </c>
@@ -4693,14 +4687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
@@ -4719,7 +4713,7 @@
     <col min="18" max="18" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4727,117 +4721,117 @@
         <v>1</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="S1" s="26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="L2" s="26" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="N2" s="26" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -4847,7 +4841,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="26"/>
@@ -4859,7 +4853,7 @@
       <c r="Q3" s="26"/>
       <c r="R3" s="26"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4867,58 +4861,58 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="E4" s="3">
         <v>500001</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L4" s="26">
         <v>70</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="R4" s="26" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -4926,58 +4920,58 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>200</v>
+        <v>151</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>201</v>
+        <v>152</v>
       </c>
       <c r="E5" s="3">
         <v>500001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L5" s="26">
         <v>70</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="R5" s="26" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -4985,58 +4979,58 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>220</v>
+        <v>155</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>222</v>
+        <v>156</v>
       </c>
       <c r="E6" s="3">
         <v>500001</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L6" s="26">
         <v>70</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="R6" s="26" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="21">
         <v>104</v>
       </c>
@@ -5044,60 +5038,60 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>221</v>
+        <v>157</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>223</v>
+        <v>158</v>
       </c>
       <c r="E7" s="3">
         <v>500001</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="L7" s="26">
         <v>70</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="R7" s="26" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File Upload Added to PageProcess
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD0C72C3-241D-4F2A-8432-C5D959F0A1C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14055" windowHeight="2055" tabRatio="613" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -35,7 +36,7 @@
     <definedName name="State">[1]Selectlists!$C$2:$C$52</definedName>
     <definedName name="waivsub">[1]Selectlists!$J$2:$J$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="250">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -61,373 +62,655 @@
     <t>Flow</t>
   </si>
   <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>TobaccoUserNo</t>
+  </si>
+  <si>
+    <t>TobaccoUserYes</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>ViewQuote</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Locators</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Male')]</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[2]/label</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[1]/label</t>
+  </si>
+  <si>
+    <t>//*[@id="mat-input-0"]</t>
+  </si>
+  <si>
+    <t>//*[@id="full_name"]</t>
+  </si>
+  <si>
+    <t>//*[@id="phone"]</t>
+  </si>
+  <si>
+    <t>//*[@id="email"]</t>
+  </si>
+  <si>
+    <t>//*[@id="getQuoteForm"]/section[4]/div/div/button</t>
+  </si>
+  <si>
+    <t>ExplicitWait</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
     <t>Click</t>
   </si>
   <si>
-    <t>Locators</t>
-  </si>
-  <si>
-    <t>ExplicitWait</t>
-  </si>
-  <si>
-    <t>101</t>
+    <t>21/11/1987</t>
+  </si>
+  <si>
+    <t>Vijay Pawar</t>
+  </si>
+  <si>
+    <t>abc@abc.com</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>21/11/1995</t>
+  </si>
+  <si>
+    <t>Abc Xyz</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>CoverageAmount</t>
+  </si>
+  <si>
+    <t>AnnualIncome</t>
+  </si>
+  <si>
+    <t>AnnualIncomePopUp</t>
+  </si>
+  <si>
+    <t>AnnualIncomeDone</t>
+  </si>
+  <si>
+    <t>PGQualification</t>
+  </si>
+  <si>
+    <t>GradQualification</t>
+  </si>
+  <si>
+    <t>QualificationDone</t>
+  </si>
+  <si>
+    <t>GetKotakLifeDiscount</t>
+  </si>
+  <si>
+    <t>Screenshot1</t>
+  </si>
+  <si>
+    <t>//input[@name="coverageAmount"]</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/section/div[3]/form/div[4]/div[2]/div</t>
+  </si>
+  <si>
+    <t>//input[@name='annual_income']</t>
+  </si>
+  <si>
+    <t>CSS = button[type='submit']</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[2]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>//*[@class="popup-main-btn"]</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Get Kotak Life Discount')]</t>
+  </si>
+  <si>
+    <t>10,00,000</t>
+  </si>
+  <si>
+    <t>im an existing kotak customer</t>
+  </si>
+  <si>
+    <t>IamCoveredUnderKotakGroupInsuranceSchemeThroughMyEmployer</t>
+  </si>
+  <si>
+    <t>SelectOrganization</t>
+  </si>
+  <si>
+    <t>ClickOrganisation</t>
+  </si>
+  <si>
+    <t>Policy no.</t>
+  </si>
+  <si>
+    <t>DiscountDone</t>
+  </si>
+  <si>
+    <t>PROCEEDTOCUSTOMIZE</t>
+  </si>
+  <si>
+    <t>YourResidentStatusIndian</t>
+  </si>
+  <si>
+    <t>YourResidentStatusNRI</t>
+  </si>
+  <si>
+    <t>PlanToVisit</t>
+  </si>
+  <si>
+    <t>ReturnDay</t>
+  </si>
+  <si>
+    <t>ResidentContinue</t>
+  </si>
+  <si>
+    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[1]/label/div/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[2]/label/div/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>[class="ng-arrow-wrapper"]</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Mahindra &amp;')]</t>
+  </si>
+  <si>
+    <t>//input[@name="policyno"]</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b done-btn"]</t>
+  </si>
+  <si>
+    <t>//button[@class="main-cta"]</t>
+  </si>
+  <si>
+    <t>//*[contains(text(),'Indian')]</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[2]/div/label[1]/div/div[2]/span</t>
+  </si>
+  <si>
+    <t>//input[@name="returnDate"]</t>
+  </si>
+  <si>
+    <t>//button[@class="popup-main-btn p-0-override mt-35-override"]</t>
+  </si>
+  <si>
+    <t>01022020</t>
+  </si>
+  <si>
+    <t>AddOnContinue</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b "]</t>
+  </si>
+  <si>
+    <t>sleep=40000</t>
+  </si>
+  <si>
+    <t>ImmediatePayout</t>
+  </si>
+  <si>
+    <t>ContinueToPayout</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-payout-details/main/section/div[1]/section/div[2]/div/div/ul/label[1]/li/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>PanDetails</t>
+  </si>
+  <si>
+    <t>PINcodeDetails</t>
+  </si>
+  <si>
+    <t>ControlKeys</t>
+  </si>
+  <si>
+    <t>ContinueButton</t>
+  </si>
+  <si>
+    <t>//input[@name="PanId"]</t>
+  </si>
+  <si>
+    <t>//input[@name="pin"]</t>
+  </si>
+  <si>
+    <t>sleep=10000</t>
+  </si>
+  <si>
+    <t>APJPV6335L</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>ContinueToPersonalDetails</t>
+  </si>
+  <si>
+    <t>TermsCheckBox</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>ProceedToPay</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>ConfirmAndProceed</t>
+  </si>
+  <si>
+    <t>ContinueToPersonal</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red btn-b"]</t>
+  </si>
+  <si>
+    <t>//*[@id="premiumAgreementForm"]/section/div/section/div[2]/div/div/div/ul/li/div[1]/label</t>
+  </si>
+  <si>
+    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[1]/div[2]/div/div[1]/div/ul/label[1]/li/div[2]/div/span</t>
+  </si>
+  <si>
+    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[2]/div/button[2]</t>
+  </si>
+  <si>
+    <t>//input[@id="ContentPlaceHolder1_rbodisclaimer_0"]</t>
+  </si>
+  <si>
+    <t>//input[@id="ContentPlaceHolder1_btnPay"]</t>
+  </si>
+  <si>
+    <t>//button[@class="btn-red"]</t>
+  </si>
+  <si>
+    <t>sleep=30000</t>
+  </si>
+  <si>
+    <t>sleep=20000</t>
+  </si>
+  <si>
+    <t>sleep=5000</t>
+  </si>
+  <si>
+    <t>input[type="checkbox"] + label:before</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>ExpiryDateMM</t>
+  </si>
+  <si>
+    <t>ExpiryDateYYYY</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>CardHolderName</t>
+  </si>
+  <si>
+    <t>MakePayment</t>
+  </si>
+  <si>
+    <t>InternetBanking</t>
+  </si>
+  <si>
+    <t>SelectYourBank</t>
+  </si>
+  <si>
+    <t>MakePayment2</t>
+  </si>
+  <si>
+    <t>Selectsuccess</t>
+  </si>
+  <si>
+    <t>Submitsuccess</t>
+  </si>
+  <si>
+    <t>ChekcingQuoteID</t>
+  </si>
+  <si>
+    <t>QuoteContinue</t>
+  </si>
+  <si>
+    <t>//*[@id="cnumber"]</t>
+  </si>
+  <si>
+    <t>//*[@id="expmon"]</t>
+  </si>
+  <si>
+    <t>//*[@id="expyr"]</t>
+  </si>
+  <si>
+    <t>//*[@id="cvv2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="cname2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="proceedForm"]</t>
+  </si>
+  <si>
+    <t>[data-value="txtBankIDBK-OTHER"]</t>
+  </si>
+  <si>
+    <t>[id="txtBankIDBK"]</t>
+  </si>
+  <si>
+    <t>[id="proceedForm"]</t>
+  </si>
+  <si>
+    <t>[class="form-control floatl"]</t>
+  </si>
+  <si>
+    <t>[name="formSubmit"]</t>
+  </si>
+  <si>
+    <t>span[class="ff-roboto-medium-override"]</t>
+  </si>
+  <si>
+    <t>[class="btn-red"]</t>
+  </si>
+  <si>
+    <t>sleep=2000</t>
+  </si>
+  <si>
+    <t>Test Bank</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>ReadValue&gt;Text</t>
+  </si>
+  <si>
+    <t>5123-4567-8901-2346</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Abc xyz</t>
+  </si>
+  <si>
+    <t>Addressline1</t>
+  </si>
+  <si>
+    <t>AdressLine2</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>LandMark</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>COntinue</t>
+  </si>
+  <si>
+    <t>YourOccupation</t>
+  </si>
+  <si>
+    <t>YourMaritalStatus</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>YourWeight</t>
+  </si>
+  <si>
+    <t>YourHeightInFeet</t>
+  </si>
+  <si>
+    <t>SelectHeightInFeet</t>
+  </si>
+  <si>
+    <t>YourHeightInInches</t>
+  </si>
+  <si>
+    <t>SelectHeightInInches</t>
+  </si>
+  <si>
+    <t>YourFatherName</t>
+  </si>
+  <si>
+    <t>YourMotherName</t>
+  </si>
+  <si>
+    <t>CONtinue</t>
+  </si>
+  <si>
+    <t>Continue12</t>
+  </si>
+  <si>
+    <t>//input[@name="addressline1"]</t>
+  </si>
+  <si>
+    <t>//input[@name="addressline2"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/input</t>
+  </si>
+  <si>
+    <t>//input[@name="landmark"]</t>
+  </si>
+  <si>
+    <t>//input[@class="ng-untouched ng-pristine ng-valid"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[1]/div[2]/div/div/label[1]/div/span[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/div/ng-select/div</t>
+  </si>
+  <si>
+    <t>[class="ng-option ng-option-marked"]</t>
+  </si>
+  <si>
+    <t>//input[@name="weight"]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[1]/ng-select/div</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[1]/ng-select/ng-dropdown-panel/div/div[2]/div[4]</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[2]/ng-select/div</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[2]/ng-select/ng-dropdown-panel/div/div[2]/div[1]</t>
+  </si>
+  <si>
+    <t>//input[@name="fatherorspouseName"]</t>
+  </si>
+  <si>
+    <t>//input[@name="motherName"]</t>
+  </si>
+  <si>
+    <t>123 new street</t>
+  </si>
+  <si>
+    <t>456 old street</t>
+  </si>
+  <si>
+    <t>mantri cosmos</t>
+  </si>
+  <si>
+    <t>suddgf sdgs</t>
+  </si>
+  <si>
+    <t>ghmfg gsgg</t>
+  </si>
+  <si>
+    <t>124 new street</t>
+  </si>
+  <si>
+    <t>457 old street</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>suddgf sdgk</t>
+  </si>
+  <si>
+    <t>ghmfg gsgl</t>
+  </si>
+  <si>
+    <t>125 new street</t>
+  </si>
+  <si>
+    <t>458 old street</t>
+  </si>
+  <si>
+    <t>126 new street</t>
+  </si>
+  <si>
+    <t>459 old street</t>
   </si>
   <si>
     <t>C:\Users\praneethm\Downloads\01T021344_Benefitillustration.pdf</t>
   </si>
   <si>
-    <t>Gender</t>
+    <t>NomineeGender</t>
+  </si>
+  <si>
+    <t>NomineeName</t>
+  </si>
+  <si>
+    <t>NomineeDOB</t>
+  </si>
+  <si>
+    <t>RelationshipWithAssured</t>
+  </si>
+  <si>
+    <t>SelectRelation</t>
+  </si>
+  <si>
+    <t>CONTinue</t>
+  </si>
+  <si>
+    <t>How Regularly Do you smoke?</t>
+  </si>
+  <si>
+    <t>Since When you have been smoking</t>
+  </si>
+  <si>
+    <t>CONTInue</t>
+  </si>
+  <si>
+    <t>CONTINue</t>
+  </si>
+  <si>
+    <t>CONTINUe</t>
+  </si>
+  <si>
+    <t>CONTINUE1</t>
+  </si>
+  <si>
+    <t>TaxResidentStatus</t>
+  </si>
+  <si>
+    <t>ResidentStatusDone</t>
   </si>
   <si>
     <t>TobaccoUser</t>
   </si>
   <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>MobileNumber</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>ViewQuote</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Male')]</t>
-  </si>
-  <si>
-    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[2]/label</t>
-  </si>
-  <si>
-    <t>//*[@id="full_name"]</t>
-  </si>
-  <si>
-    <t>//*[@id="phone"]</t>
-  </si>
-  <si>
-    <t>//*[@id="getQuoteForm"]/section[4]/div/div/button</t>
-  </si>
-  <si>
-    <t>21/11/1987</t>
-  </si>
-  <si>
-    <t>Vijay Pawar</t>
-  </si>
-  <si>
-    <t>CoverageAmount</t>
-  </si>
-  <si>
-    <t>im an existing kotak customer</t>
-  </si>
-  <si>
-    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[1]/label/div/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b done-btn"]</t>
-  </si>
-  <si>
-    <t>//input[@name="coverageAmount"]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/section/div[3]/form/div[4]/div[2]/div</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Get Kotak Life Discount')]</t>
-  </si>
-  <si>
-    <t>GetKotakLifeDiscount</t>
-  </si>
-  <si>
-    <t>//*[@id="mat-input-0"]</t>
-  </si>
-  <si>
-    <t>//*[@id="email"]</t>
-  </si>
-  <si>
-    <t>abc@abc.com</t>
-  </si>
-  <si>
-    <t>Policy no.</t>
-  </si>
-  <si>
-    <t>//input[@name="policyno"]</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Indian')]</t>
-  </si>
-  <si>
-    <t>//button[@class="popup-main-btn p-0-override mt-35-override"]</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b "]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-payout-details/main/section/div[1]/section/div[2]/div/div/ul/label[1]/li/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>ImmediatePayout</t>
-  </si>
-  <si>
-    <t>//button[@class="main-cta"]</t>
-  </si>
-  <si>
-    <t>PROCEEDTOCUSTOMIZE</t>
-  </si>
-  <si>
-    <t>AnnualIncomePopUp</t>
-  </si>
-  <si>
-    <t>//input[@name='annual_income']</t>
-  </si>
-  <si>
-    <t>AnnualIncome</t>
-  </si>
-  <si>
-    <t>10,00,000</t>
-  </si>
-  <si>
-    <t>//*[@class="popup-main-btn"]</t>
-  </si>
-  <si>
-    <t>PGQualification</t>
-  </si>
-  <si>
-    <t>CSS = button[type='submit']</t>
-  </si>
-  <si>
-    <t>AnnualIncomeDone</t>
-  </si>
-  <si>
-    <t>QualificationDone</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[1]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>DiscountDone</t>
-  </si>
-  <si>
-    <t>AddOnContinue</t>
-  </si>
-  <si>
-    <t>ResidentContinue</t>
-  </si>
-  <si>
-    <t>ContinueToPayout</t>
-  </si>
-  <si>
-    <t>//input[@name="PanId"]</t>
-  </si>
-  <si>
-    <t>APJPV6335L</t>
-  </si>
-  <si>
-    <t>//input[@name="pin"]</t>
-  </si>
-  <si>
-    <t>PINcodeDetails</t>
-  </si>
-  <si>
-    <t>ContinueButton</t>
-  </si>
-  <si>
-    <t>PanDetails</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red btn-b"]</t>
-  </si>
-  <si>
-    <t>ContinueToPersonalDetails</t>
-  </si>
-  <si>
-    <t>TermsCheckBox</t>
-  </si>
-  <si>
-    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[1]/div[2]/div/div[1]/div/ul/label[1]/li/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>PaymentMode</t>
-  </si>
-  <si>
-    <t>ProceedToPay</t>
-  </si>
-  <si>
-    <t>//button[@class="btn-red"]</t>
-  </si>
-  <si>
-    <t>ContinueToPersonal</t>
-  </si>
-  <si>
-    <t>ControlKeys</t>
-  </si>
-  <si>
-    <t>Tab</t>
-  </si>
-  <si>
-    <t>sleep=30000</t>
-  </si>
-  <si>
-    <t>//input[@name="addressline1"]</t>
-  </si>
-  <si>
-    <t>Addressline1</t>
-  </si>
-  <si>
-    <t>//input[@name="addressline2"]</t>
-  </si>
-  <si>
-    <t>AdressLine2</t>
-  </si>
-  <si>
-    <t>PinCode</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/input</t>
-  </si>
-  <si>
-    <t>LandMark</t>
-  </si>
-  <si>
-    <t>//input[@name="landmark"]</t>
-  </si>
-  <si>
-    <t>//input[@class="ng-untouched ng-pristine ng-valid"]</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>COntinue</t>
-  </si>
-  <si>
-    <t>input[type="checkbox"] + label:before</t>
-  </si>
-  <si>
-    <t>123 new street</t>
-  </si>
-  <si>
-    <t>456 old street</t>
-  </si>
-  <si>
-    <t>mantri cosmos</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>YourOccupation</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[1]/div[2]/div/div/label[1]/div/span[1]</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[2]/div[1]/div/div/ng-select/div</t>
-  </si>
-  <si>
-    <t>YourMaritalStatus</t>
-  </si>
-  <si>
-    <t>Single</t>
-  </si>
-  <si>
-    <t>//input[@name="weight"]</t>
-  </si>
-  <si>
-    <t>YourWeight</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[1]/ng-select/div</t>
-  </si>
-  <si>
-    <t>//input[@name="fatherorspouseName"]</t>
-  </si>
-  <si>
-    <t>YourFatherName</t>
-  </si>
-  <si>
-    <t>//input[@name="motherName"]</t>
-  </si>
-  <si>
-    <t>YourMotherName</t>
-  </si>
-  <si>
-    <t>CONtinue</t>
-  </si>
-  <si>
-    <t>SelectHeightInFeet</t>
-  </si>
-  <si>
-    <t>SelectHeightInInches</t>
-  </si>
-  <si>
-    <t>YourHeightInFeet</t>
-  </si>
-  <si>
-    <t>YourHeightInInches</t>
-  </si>
-  <si>
-    <t>suddgf sdgs</t>
-  </si>
-  <si>
-    <t>ghmfg gsgg</t>
+    <t>AadharDetails</t>
+  </si>
+  <si>
+    <t>IAgree1</t>
+  </si>
+  <si>
+    <t>InsuredOrProposer</t>
+  </si>
+  <si>
+    <t>IAgree2</t>
+  </si>
+  <si>
+    <t>ProposalForm</t>
+  </si>
+  <si>
+    <t>ThirdPartyPayment</t>
+  </si>
+  <si>
+    <t>IAgree3</t>
+  </si>
+  <si>
+    <t>Continue2</t>
   </si>
   <si>
     <t>//*[@id="nomineeForm"]/section[1]/div[2]/div[1]/div[1]/div/div/label[2]/div/span[1]</t>
   </si>
   <si>
-    <t>NomineeGender</t>
-  </si>
-  <si>
     <t>//input[@class="form-control ng-untouched ng-pristine ng-invalid"]</t>
   </si>
   <si>
-    <t>//*[@id="premiumAgreementForm"]/section/div/section/div[2]/div/div/div/ul/li/div[1]/label</t>
-  </si>
-  <si>
-    <t>Window</t>
-  </si>
-  <si>
-    <t>//*[@id="paymentmethodForm"]/section[2]/div/section[2]/div/button[2]</t>
-  </si>
-  <si>
-    <t>//*[@id="personalDetailsForm"]/div/div[3]/div[1]/div/div/div[2]/ng-select/div</t>
-  </si>
-  <si>
-    <t>NomineeName</t>
-  </si>
-  <si>
-    <t>NomineeDOB</t>
-  </si>
-  <si>
     <t>//input[@class="form-control input-date ng-untouched ng-pristine ng-invalid"]</t>
   </si>
   <si>
     <t>//*[@bindlabel="name"]</t>
   </si>
   <si>
-    <t>RelationshipWithAssured</t>
-  </si>
-  <si>
     <t>//*[@class="ng-option ng-star-inserted ng-option-marked"]</t>
   </si>
   <si>
-    <t>SelectRelation</t>
-  </si>
-  <si>
-    <t>CONTinue</t>
-  </si>
-  <si>
-    <t>CONTInue</t>
-  </si>
-  <si>
-    <t>CONTINue</t>
+    <t>//*[contains(text(),'Once a week')]</t>
+  </si>
+  <si>
+    <t>//*[@class="ng-select-container ng-has-value"]</t>
   </si>
   <si>
     <t>//*[@id="highriskForm"]/main/section/div/section/div/button[2]</t>
@@ -436,380 +719,101 @@
     <t>//*[@id="questionsForm"]/main/section/div/section/div/button[2]</t>
   </si>
   <si>
-    <t>CONTINUe</t>
-  </si>
-  <si>
     <t>//button[@class="popup-main-btn"]</t>
   </si>
   <si>
-    <t>CONTINUE1</t>
-  </si>
-  <si>
-    <t>TaxResidentStatus</t>
-  </si>
-  <si>
     <t>//*[@id="discountform"]/section/div/section[1]/div/div/div[1]/div/ul/li[1]/label/div/div[1]/div/span</t>
   </si>
   <si>
-    <t>ResidentStatusDone</t>
-  </si>
-  <si>
     <t>//*[@for="tandc"]</t>
   </si>
   <si>
     <t>//*[@for="tand8"]</t>
   </si>
   <si>
-    <t>AadharDetails</t>
-  </si>
-  <si>
-    <t>InsuredOrProposer</t>
-  </si>
-  <si>
-    <t>ProposalForm</t>
-  </si>
-  <si>
-    <t>ThirdPartyPayment</t>
-  </si>
-  <si>
-    <t>Continue2</t>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[3]/div[2]/div[2]/div[2]/button</t>
   </si>
   <si>
     <t>//*[@for="tand1"]</t>
   </si>
   <si>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[1]/div[2]/div[2]/div[2]/button</t>
+  </si>
+  <si>
     <t>//*[@for="tand3"]</t>
   </si>
   <si>
     <t>//*[@for="tand5"]</t>
   </si>
   <si>
+    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[2]/div[2]/div[2]/div[2]/button</t>
+  </si>
+  <si>
     <t>//button[@class="ff-roboto-bold-override btn-red btn-b lts-30-override"]</t>
   </si>
   <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[3]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree1</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[1]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree2</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-pay-premium-agreement/app-normal-modal[2]/div[2]/div[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>IAgree3</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[1]/ng-select/ng-dropdown-panel/div/div[2]/div[4]</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-personal-details/main/section/div/section/form/div/div[3]/div[1]/div/div/div[2]/ng-select/ng-dropdown-panel/div/div[2]/div[1]</t>
-  </si>
-  <si>
-    <t>sleep=10000</t>
+    <t>FileUpload</t>
+  </si>
+  <si>
+    <t>FileUpload1</t>
+  </si>
+  <si>
+    <t>FileUpload2</t>
+  </si>
+  <si>
+    <t>FileUpload3</t>
+  </si>
+  <si>
+    <t>FileUpload4</t>
+  </si>
+  <si>
+    <t>FileUpload5</t>
+  </si>
+  <si>
+    <t>FileUpload6</t>
+  </si>
+  <si>
+    <t>UploadDone</t>
   </si>
   <si>
     <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[1]/div[2]/button</t>
   </si>
   <si>
-    <t>Browse1</t>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[2]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[3]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[4]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[5]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[6]/div[2]/button</t>
+  </si>
+  <si>
+    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[7]/div[2]/button</t>
+  </si>
+  <si>
+    <t>[class="btn-red text-uppercase"]</t>
+  </si>
+  <si>
+    <t>C:\Users\Andrew.Kroner\Desktop\01T225928_Benefitillustration.pdf</t>
   </si>
   <si>
     <t>C:\Users\praneethm\Downloads\01T021466_Benefitillustration.pdf</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[2]/div[2]/button</t>
-  </si>
-  <si>
-    <t>Browse2</t>
-  </si>
-  <si>
-    <t>Browse3</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[3]/div[2]/button</t>
-  </si>
-  <si>
-    <t>Browse4</t>
-  </si>
-  <si>
-    <t>Browse5</t>
-  </si>
-  <si>
-    <t>//input[@id="ContentPlaceHolder1_rbodisclaimer_0"]</t>
-  </si>
-  <si>
-    <t>Confirmation</t>
-  </si>
-  <si>
-    <t>//input[@id="ContentPlaceHolder1_btnPay"]</t>
-  </si>
-  <si>
-    <t>ConfirmAndProceed</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>ExpiryDateMM</t>
-  </si>
-  <si>
-    <t>ExpiryDateYYYY</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>CardHolderName</t>
-  </si>
-  <si>
-    <t>MakePayment</t>
-  </si>
-  <si>
-    <t>5123-4567-8901-2346</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>Abc xyz</t>
-  </si>
-  <si>
-    <t>//*[@id="cnumber"]</t>
-  </si>
-  <si>
-    <t>//*[@id="expmon"]</t>
-  </si>
-  <si>
-    <t>//*[@id="expyr"]</t>
-  </si>
-  <si>
-    <t>//*[@id="cvv2"]</t>
-  </si>
-  <si>
-    <t>//*[@id="cname2"]</t>
-  </si>
-  <si>
-    <t>//*[@id="proceedForm"]</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>Abc Xyz</t>
-  </si>
-  <si>
-    <t>TobaccoUserNo</t>
-  </si>
-  <si>
-    <t>TobaccoUserYes</t>
-  </si>
-  <si>
-    <t>GradQualification</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[1]/label[2]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>124 new street</t>
-  </si>
-  <si>
-    <t>457 old street</t>
-  </si>
-  <si>
-    <t>ghmfg gsgl</t>
-  </si>
-  <si>
-    <t>suddgf sdgk</t>
-  </si>
-  <si>
-    <t>How Regularly Do you smoke?</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Once a week')]</t>
-  </si>
-  <si>
-    <t>Since When you have been smoking</t>
-  </si>
-  <si>
-    <t>//*[@class="ng-select-container ng-has-value"]</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>SelectOrganization</t>
-  </si>
-  <si>
-    <t>YourResidentStatusIndian</t>
-  </si>
-  <si>
-    <t>YourResidentStatusNRI</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-quotation/div[2]/div/div[2]/div[2]/div/label[1]/div/div[2]/span</t>
-  </si>
-  <si>
-    <t>PlanToVisit</t>
-  </si>
-  <si>
-    <t>//input[@name="returnDate"]</t>
-  </si>
-  <si>
-    <t>ReturnDay</t>
-  </si>
-  <si>
-    <t>01022020</t>
-  </si>
-  <si>
-    <t>21/11/1995</t>
-  </si>
-  <si>
-    <t>125 new street</t>
-  </si>
-  <si>
-    <t>126 new street</t>
-  </si>
-  <si>
-    <t>458 old street</t>
-  </si>
-  <si>
-    <t>459 old street</t>
-  </si>
-  <si>
-    <t>Screenshot</t>
-  </si>
-  <si>
-    <t>Screenshot1</t>
-  </si>
-  <si>
-    <t>[data-value="txtBankIDBK-OTHER"]</t>
-  </si>
-  <si>
-    <t>InternetBanking</t>
-  </si>
-  <si>
-    <t>SelectYourBank</t>
-  </si>
-  <si>
-    <t>[id="txtBankIDBK"]</t>
-  </si>
-  <si>
-    <t>Test Bank</t>
-  </si>
-  <si>
-    <t>[id="proceedForm"]</t>
-  </si>
-  <si>
-    <t>sleep=20000</t>
-  </si>
-  <si>
-    <t>MakePayment2</t>
-  </si>
-  <si>
-    <t>[class="form-control floatl"]</t>
-  </si>
-  <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>[name="formSubmit"]</t>
-  </si>
-  <si>
-    <t>span[class="ff-roboto-medium-override"]</t>
-  </si>
-  <si>
-    <t>ChekcingQuoteID</t>
-  </si>
-  <si>
-    <t>[class="btn-red"]</t>
-  </si>
-  <si>
-    <t>QuoteContinue</t>
-  </si>
-  <si>
-    <t>Selectsuccess</t>
-  </si>
-  <si>
-    <t>Submitsuccess</t>
-  </si>
-  <si>
-    <t>ReadValue&gt;Text</t>
-  </si>
-  <si>
-    <t>Continue12</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[4]/div[2]/button</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[5]/div[2]/button</t>
-  </si>
-  <si>
-    <t>Browse6</t>
-  </si>
-  <si>
-    <t>Browse7</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[6]/div[2]/button</t>
-  </si>
-  <si>
-    <t>/html/body/app-root/main/app-document-processing/app-document-processing-web/main/section/div/section[1]/div[2]/div/div/ul/li[7]/div[2]/button</t>
-  </si>
-  <si>
-    <t>[class="btn-red text-uppercase"]</t>
-  </si>
-  <si>
-    <t>UploadDone</t>
-  </si>
-  <si>
-    <t>[class="ng-option ng-option-marked"]</t>
-  </si>
-  <si>
-    <t>sleep=5000</t>
-  </si>
-  <si>
-    <t>sleep=2000</t>
-  </si>
-  <si>
-    <t>IamCoveredUnderKotakGroupInsuranceSchemeThroughMyEmployer</t>
-  </si>
-  <si>
-    <t>//*[@id="discountform"]/section/div/section[1]/div[2]/div/div[1]/div/ul/li[2]/label/div/div[2]/div/span</t>
-  </si>
-  <si>
-    <t>//*[contains(text(),'Mahindra &amp;')]</t>
-  </si>
-  <si>
-    <t>ClickOrganisation</t>
-  </si>
-  <si>
-    <t>[class="ng-arrow-wrapper"]</t>
-  </si>
-  <si>
-    <t>//*[@id="getQuoteForm"]/section[1]/div/div/div[2]/div/div[1]/label</t>
-  </si>
-  <si>
-    <t>sleep=40000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1145,7 +1149,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1810,14 +1814,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -1833,7 +1837,7 @@
     <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1841,59 +1845,59 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="28" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="F1" s="42" t="s">
+      <c r="J1" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="L1" s="41"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="28" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="46" t="s">
-        <v>210</v>
-      </c>
-      <c r="L1" s="41"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="G2" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="54" t="s">
-        <v>247</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="28" t="s">
+      <c r="H2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="I2" s="28" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>31</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>19</v>
@@ -1901,9 +1905,9 @@
       <c r="K2" s="23"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -1916,135 +1920,135 @@
       <c r="K3" s="23"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="43" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="27" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H4" s="26">
         <v>9999999999</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K4" s="23"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="43" t="s">
-        <v>181</v>
+        <v>27</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>205</v>
+        <v>28</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="H5" s="26">
         <v>9999999999</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="44" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="29" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H6" s="22">
         <v>9999999999</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="45" t="s">
-        <v>196</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>205</v>
+        <v>28</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>182</v>
+        <v>29</v>
       </c>
       <c r="H7" s="26">
         <v>9999999999</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="40"/>
       <c r="B8" s="10"/>
       <c r="C8" s="5"/>
@@ -2058,7 +2062,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="40"/>
       <c r="B9" s="10"/>
       <c r="C9" s="5"/>
@@ -2072,7 +2076,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="37"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="40"/>
       <c r="B10" s="10"/>
       <c r="C10" s="5"/>
@@ -2086,7 +2090,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="40"/>
       <c r="B11" s="10"/>
       <c r="C11" s="5"/>
@@ -2100,7 +2104,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="40"/>
       <c r="B12" s="10"/>
       <c r="C12" s="5"/>
@@ -2114,7 +2118,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="40"/>
       <c r="B13" s="10"/>
       <c r="C13" s="5"/>
@@ -2128,7 +2132,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="E16" s="23"/>
     </row>
   </sheetData>
@@ -2138,14 +2142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
@@ -2166,7 +2170,7 @@
     <col min="18" max="18" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2174,161 +2178,161 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>190</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>116</v>
+        <v>191</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>119</v>
+        <v>192</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>122</v>
+        <v>194</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>124</v>
+        <v>198</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>127</v>
+        <v>199</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>129</v>
+        <v>200</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>130</v>
+        <v>201</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>132</v>
+        <v>202</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>135</v>
+        <v>204</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>136</v>
+        <v>206</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>147</v>
+        <v>207</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>149</v>
+        <v>210</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>110</v>
+        <v>213</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>117</v>
+        <v>214</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>126</v>
+        <v>220</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>128</v>
+        <v>221</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>134</v>
+        <v>224</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>144</v>
+        <v>225</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>146</v>
+        <v>227</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>141</v>
+        <v>228</v>
       </c>
       <c r="W2" s="2"/>
       <c r="X2" s="2" t="s">
-        <v>142</v>
+        <v>229</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2358,7 +2362,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -2375,56 +2379,56 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="24"/>
       <c r="K4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="W4" s="3">
         <v>0</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -2432,70 +2436,70 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
         <v>12011987</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="W5" s="2">
         <v>0</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -2503,7 +2507,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
@@ -2512,56 +2516,56 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="24"/>
       <c r="K6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="W6" s="3">
         <v>0</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="14">
         <v>104</v>
       </c>
@@ -2578,20 +2582,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="125.5703125" customWidth="1"/>
+    <col min="4" max="4" width="126.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2599,70 +2608,70 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>233</v>
       </c>
       <c r="E1" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>235</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>236</v>
       </c>
       <c r="H1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="I1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="J1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="K1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="F2" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G2" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="H2" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="I2" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="J2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -2670,34 +2679,34 @@
         <v>11</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>155</v>
+        <v>248</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -2712,7 +2721,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -2720,28 +2729,28 @@
         <v>11</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="H6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="I6" s="47" t="s">
-        <v>155</v>
+        <v>249</v>
       </c>
       <c r="J6" s="48" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -2753,14 +2762,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -2774,7 +2783,7 @@
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -2782,66 +2791,66 @@
         <v>1</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>185</v>
+        <v>37</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1">
       <c r="A2" s="28" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>43</v>
       </c>
       <c r="F2" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1">
       <c r="A3" s="28" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28">
@@ -2855,7 +2864,7 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1">
       <c r="A4" s="28">
         <v>101</v>
       </c>
@@ -2866,26 +2875,26 @@
         <v>25000000</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="H4" s="28"/>
       <c r="I4" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="28">
         <v>102</v>
       </c>
@@ -2896,24 +2905,24 @@
         <v>25000000</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E5" s="26">
         <v>200000</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G5" s="28"/>
       <c r="H5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="28">
         <v>103</v>
       </c>
@@ -2924,26 +2933,26 @@
         <v>25000000</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E6" s="28">
         <v>1000000</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="31">
         <v>104</v>
       </c>
@@ -2954,20 +2963,20 @@
         <v>25000000</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E7" s="26">
         <v>200000</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I7" s="28" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J7" s="28"/>
     </row>
@@ -2977,14 +2986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AO14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -3024,7 +3033,7 @@
     <col min="40" max="40" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3032,40 +3041,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>242</v>
+        <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>245</v>
+        <v>53</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>199</v>
+        <v>58</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>203</v>
+        <v>60</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="10"/>
@@ -3095,46 +3104,46 @@
       <c r="AN1" s="10"/>
       <c r="AO1" s="5"/>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>243</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>246</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>244</v>
+        <v>65</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>186</v>
+        <v>46</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>202</v>
+        <v>71</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
@@ -3164,9 +3173,9 @@
       <c r="AN2" s="10"/>
       <c r="AO2" s="5"/>
     </row>
-    <row r="3" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="2" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3217,7 +3226,7 @@
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
     </row>
-    <row r="4" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" s="2" customFormat="1">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3225,7 +3234,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -3234,19 +3243,19 @@
         <v>1974551</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
@@ -3276,7 +3285,7 @@
       <c r="AN4" s="10"/>
       <c r="AO4" s="5"/>
     </row>
-    <row r="5" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" s="2" customFormat="1">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -3290,16 +3299,16 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
@@ -3329,7 +3338,7 @@
       <c r="AN5" s="10"/>
       <c r="AO5" s="5"/>
     </row>
-    <row r="6" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" s="2" customFormat="1">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -3338,29 +3347,29 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
@@ -3390,7 +3399,7 @@
       <c r="AN6" s="10"/>
       <c r="AO6" s="5"/>
     </row>
-    <row r="7" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" s="2" customFormat="1">
       <c r="A7" s="3">
         <v>104</v>
       </c>
@@ -3404,20 +3413,20 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>204</v>
+        <v>73</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
@@ -3447,7 +3456,7 @@
       <c r="AN7" s="10"/>
       <c r="AO7" s="5"/>
     </row>
-    <row r="8" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" s="2" customFormat="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -3490,7 +3499,7 @@
       <c r="AN8" s="10"/>
       <c r="AO8" s="5"/>
     </row>
-    <row r="9" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" s="2" customFormat="1">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -3533,7 +3542,7 @@
       <c r="AN9" s="10"/>
       <c r="AO9" s="5"/>
     </row>
-    <row r="10" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" s="2" customFormat="1">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -3576,7 +3585,7 @@
       <c r="AN10" s="5"/>
       <c r="AO10" s="5"/>
     </row>
-    <row r="11" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -3619,7 +3628,7 @@
       <c r="AN11" s="10"/>
       <c r="AO11" s="5"/>
     </row>
-    <row r="12" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3662,7 +3671,7 @@
       <c r="AN12" s="10"/>
       <c r="AO12" s="5"/>
     </row>
-    <row r="13" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" s="2" customFormat="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -3705,7 +3714,7 @@
       <c r="AN13" s="10"/>
       <c r="AO13" s="5"/>
     </row>
-    <row r="14" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" s="2" customFormat="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -3750,7 +3759,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="O5 Q5 V5 AB4:AC7 AB13:AC13 Q7 V7 O7"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="O5 Q5 V5 AB4:AC7 AB13:AC13 Q7 V7 O7" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3758,21 +3767,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3780,28 +3789,28 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -3809,10 +3818,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -3820,10 +3829,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -3831,10 +3840,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="14">
         <v>104</v>
       </c>
@@ -3842,7 +3851,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3851,14 +3860,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AP10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
@@ -3899,7 +3908,7 @@
     <col min="38" max="38" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3907,10 +3916,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -3951,16 +3960,16 @@
       <c r="AO1" s="49"/>
       <c r="AP1" s="49"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -4001,9 +4010,9 @@
       <c r="AO2" s="49"/>
       <c r="AP2" s="49"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -4047,7 +4056,7 @@
       <c r="AO3" s="49"/>
       <c r="AP3" s="49"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4055,10 +4064,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -4099,7 +4108,7 @@
       <c r="AO4" s="49"/>
       <c r="AP4" s="49"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -4107,10 +4116,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4151,7 +4160,7 @@
       <c r="AO5" s="49"/>
       <c r="AP5" s="49"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -4159,10 +4168,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -4203,7 +4212,7 @@
       <c r="AO6" s="49"/>
       <c r="AP6" s="49"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42">
       <c r="A7" s="3">
         <v>104</v>
       </c>
@@ -4211,10 +4220,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4255,7 +4264,7 @@
       <c r="AO7" s="49"/>
       <c r="AP7" s="49"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42">
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -4295,7 +4304,7 @@
       <c r="AO8" s="49"/>
       <c r="AP8" s="49"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42">
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -4335,7 +4344,7 @@
       <c r="AO9" s="49"/>
       <c r="AP9" s="49"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42">
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -4382,14 +4391,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
@@ -4399,7 +4408,7 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4407,56 +4416,56 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.5" customHeight="1">
       <c r="A2" s="12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="12" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="13" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" customHeight="1">
       <c r="A4" s="13">
         <v>101</v>
       </c>
@@ -4464,22 +4473,22 @@
         <v>6</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D4" s="13">
         <v>500072</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -4487,22 +4496,22 @@
         <v>6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D5" s="13">
         <v>500072</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -4510,22 +4519,22 @@
         <v>6</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D6" s="13">
         <v>500072</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>104</v>
       </c>
@@ -4533,40 +4542,40 @@
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D7" s="13">
         <v>500072</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -4579,14 +4588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -4600,7 +4609,7 @@
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4608,74 +4617,74 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>163</v>
+        <v>94</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>218</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>240</v>
+        <v>106</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -4683,7 +4692,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4691,29 +4700,29 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="10">
         <v>102</v>
       </c>
@@ -4721,25 +4730,25 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="10">
         <v>103</v>
       </c>
@@ -4747,29 +4756,29 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="14">
         <v>104</v>
       </c>
@@ -4777,27 +4786,27 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="D13" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -4807,14 +4816,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
@@ -4833,7 +4842,7 @@
     <col min="16" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4841,93 +4850,93 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>171</v>
+        <v>113</v>
       </c>
       <c r="I1" s="52" t="s">
-        <v>213</v>
+        <v>114</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>219</v>
+        <v>116</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>227</v>
+        <v>117</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>228</v>
+        <v>118</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>224</v>
+        <v>119</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>180</v>
+        <v>126</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>212</v>
+        <v>127</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>215</v>
+        <v>128</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>217</v>
+        <v>129</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>220</v>
+        <v>130</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>222</v>
+        <v>131</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>223</v>
+        <v>132</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -4942,13 +4951,13 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>240</v>
+        <v>106</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -4962,28 +4971,28 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>216</v>
+        <v>135</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>221</v>
+        <v>136</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>229</v>
+        <v>137</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="3">
         <v>102</v>
       </c>
@@ -4991,10 +5000,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="E5" s="3">
         <v>2020</v>
@@ -5003,10 +5012,10 @@
         <v>123</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -5016,7 +5025,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -5030,28 +5039,28 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>216</v>
+        <v>135</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L6" s="53" t="s">
-        <v>221</v>
+        <v>136</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>229</v>
+        <v>137</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="15">
         <v>104</v>
       </c>
@@ -5079,14 +5088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H5" workbookViewId="0">
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" customWidth="1"/>
@@ -5107,7 +5116,7 @@
     <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5115,123 +5124,123 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
       <c r="N1" s="19" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="O1" s="19" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="R1" s="19" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>101</v>
+        <v>157</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>159</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>239</v>
+        <v>166</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>94</v>
+        <v>167</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>96</v>
+        <v>168</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="Q2" s="19" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>99</v>
+        <v>173</v>
       </c>
       <c r="S2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="T2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5241,7 +5250,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="19"/>
@@ -5253,7 +5262,7 @@
       <c r="Q3" s="19"/>
       <c r="R3" s="19"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -5261,57 +5270,57 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L4" s="19">
         <v>70</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="19" t="s">
-        <v>106</v>
+        <v>177</v>
       </c>
       <c r="R4" s="19" t="s">
-        <v>107</v>
+        <v>178</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -5319,58 +5328,58 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E5" s="3">
         <v>500001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L5" s="19">
         <v>70</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="R5" s="19" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>103</v>
       </c>
@@ -5378,61 +5387,61 @@
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="E6" s="3">
         <v>500001</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L6" s="19">
         <v>70</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="19" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="R6" s="19" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="14">
         <v>104</v>
       </c>
@@ -5440,60 +5449,60 @@
         <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3">
         <v>500001</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>87</v>
+        <v>176</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L7" s="19">
         <v>70</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to the test data
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\VMSeleniumFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1252E347-4E57-41DD-8302-127D42AE6589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A06A70-B022-4281-8CE2-61D8863C06AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="605" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4033" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4227" uniqueCount="722">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -1952,9 +1952,6 @@
     <t>36</t>
   </si>
   <si>
-    <t>PDFText&gt;5,050 0 5,051</t>
-  </si>
-  <si>
     <t>PDFText&gt;5,050 0 5,052</t>
   </si>
   <si>
@@ -2094,6 +2091,138 @@
   </si>
   <si>
     <t>[class="quoteClass"] strong</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Existing Customer+Yes||Installment First Year Premium (including Step-Up Option+fee, if any) without GST (Rs.) :+5,051</t>
+  </si>
+  <si>
+    <t>12/12/1987</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,925     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,925     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 4,632 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 4,632</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,302     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,302     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,536 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,536</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 433,900   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 433,900   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 512,002 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 512,002</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 13,931    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 13,931    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 16,439 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 16,439</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 7,889     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 7,889     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 9,309 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 9,309</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,825     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,825     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 4,514 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 4,514</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 6,625     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 6,625     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 7,818 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 7,818</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,205     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,205     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,422 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,422</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 971       || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 971       || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,146 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,146</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 5,346     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 5,346     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 6,308 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 6,308</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 200,000   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 200,000   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 236,000 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 236,000</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 37,356    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 37,356    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 44,080 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 44,080</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 58,794    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 58,794    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 69,377 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 69,377</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 424       || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 424       || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 500 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 500</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 248,016   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 248,016   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 292,659 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 292,659</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 10,875    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 10,875    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 12,833 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 12,833</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 403,704   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 403,704   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 476,371 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 476,371</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 34,933    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 34,933    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 41,221 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 41,221</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 2,256,200 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 2,256,200 || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 2,662,316 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 2,662,316</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 705,000   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 705,000   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 831,900 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 831,900</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 15,391    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 15,391    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 18,161 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 18,161</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 56,400    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 56,400    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 66,552 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 66,552</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 296,190   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 296,190   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 349,504 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 349,504</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,150,250 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,150,250 || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,357,295 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,357,295</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,294     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,294     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,527 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,527</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 928       || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 928       || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 1,095 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 1,095</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,621     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,621     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 4,273 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 4,273</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 7,556     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 7,556     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 8,916 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 8,916</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 10,540    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 10,540    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 12,437 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 12,437</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 5,051     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 5,051     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 5,960 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 5,960</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 178,125   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 178,125   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 210,188 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 210,188</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 5,398     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 5,398     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 6,370 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 6,370</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 6,217     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 6,217     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 7,336 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 7,336</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 669,600   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 669,600   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 790,128 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 790,128</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,702     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,702     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 4,368 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 4,368</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 17,688    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 17,688    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 20,872 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 20,872</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 31,416    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 31,416    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 37,071 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 37,071</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 14,863    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 14,863    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 17,538 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 17,538</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 690,000   || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 690,000   || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 814,200 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 814,200</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 51,400    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 51,400    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 60,652 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 60,652</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 19,975    || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 19,975    || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 23,571 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 23,571</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,010     || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,010     || Installment First Year Premium (including Step-Up Option + fee, if any) without GST (Rs.) : + 3,552 || Installment Second Year onwards Premium (including Step-+ Up Option fee, if any) without GST (Rs.) + 3,552</t>
   </si>
 </sst>
 </file>
@@ -3515,8 +3644,8 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A108:A121"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6941,8 +7070,8 @@
       <c r="F89" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H89" s="115">
-        <v>32123</v>
+      <c r="H89" s="116" t="s">
+        <v>679</v>
       </c>
       <c r="K89" s="110" t="s">
         <v>532</v>
@@ -9108,10 +9237,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>642</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>643</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
@@ -9166,10 +9295,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>644</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>645</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
@@ -9224,10 +9353,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>646</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>647</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
@@ -9282,10 +9411,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>648</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
@@ -9340,10 +9469,10 @@
         <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>650</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>651</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
@@ -9398,10 +9527,10 @@
         <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>652</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>653</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -9456,10 +9585,10 @@
         <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>654</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>655</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -9514,10 +9643,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>656</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>657</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
@@ -9572,10 +9701,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>658</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>659</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
@@ -9630,10 +9759,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>660</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>661</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
@@ -9688,10 +9817,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>662</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>663</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
@@ -10641,8 +10770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280E1A22-750B-4771-AF4C-76F857DCAC92}">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10736,7 +10865,7 @@
         <v>436</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -11034,7 +11163,7 @@
         <v>501</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="M10" s="7">
         <v>0</v>
@@ -11081,7 +11210,7 @@
         <v>501</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M11" s="7">
         <v>0</v>
@@ -11128,7 +11257,7 @@
         <v>501</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="M12" s="7">
         <v>0</v>
@@ -11175,7 +11304,7 @@
         <v>501</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="M13" s="7">
         <v>0</v>
@@ -11222,7 +11351,7 @@
         <v>501</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="M14" s="7">
         <v>0</v>
@@ -11269,7 +11398,7 @@
         <v>501</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="M15" s="7">
         <v>0</v>
@@ -11316,7 +11445,7 @@
         <v>501</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="M16" s="7">
         <v>0</v>
@@ -11363,7 +11492,7 @@
         <v>501</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="M17" s="7">
         <v>0</v>
@@ -11410,7 +11539,7 @@
         <v>501</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M18" s="7">
         <v>0</v>
@@ -11457,7 +11586,7 @@
         <v>501</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M19" s="7">
         <v>0</v>
@@ -11504,7 +11633,7 @@
         <v>501</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="M20" s="7">
         <v>0</v>
@@ -11551,7 +11680,7 @@
         <v>501</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="M21" s="7">
         <v>0</v>
@@ -11905,9 +12034,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V72" sqref="V72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17763,7 +17892,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21587,7 +21716,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22224,6 +22353,9 @@
       </c>
       <c r="B60" s="7">
         <v>5</v>
+      </c>
+      <c r="C60" s="91" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -24908,7 +25040,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:A70"/>
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25691,9 +25823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AA71"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S59" sqref="S59"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25701,12 +25833,12 @@
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
@@ -25714,7 +25846,7 @@
     <col min="14" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27" customWidth="1"/>
+    <col min="18" max="18" width="27.42578125" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" customWidth="1"/>
     <col min="20" max="20" width="26.140625" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" customWidth="1"/>
@@ -26256,12 +26388,24 @@
       <c r="M11" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="N11" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P11" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="S11" s="7">
+        <v>0</v>
+      </c>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
@@ -26288,12 +26432,24 @@
       <c r="M12" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
+      <c r="N12" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0</v>
+      </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
@@ -26332,12 +26488,24 @@
       <c r="M13" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="N13" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P13" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="S13" s="7">
+        <v>0</v>
+      </c>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
@@ -26364,12 +26532,24 @@
       <c r="M14" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="N14" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P14" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="S14" s="7">
+        <v>0</v>
+      </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
@@ -26396,12 +26576,24 @@
       <c r="M15" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
+      <c r="N15" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P15" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="S15" s="7">
+        <v>0</v>
+      </c>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -26440,12 +26632,24 @@
       <c r="M16" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
+      <c r="N16" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P16" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0</v>
+      </c>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
@@ -26472,12 +26676,24 @@
       <c r="M17" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="S17" s="3"/>
+      <c r="N17" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P17" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="S17" s="7">
+        <v>0</v>
+      </c>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -26504,12 +26720,24 @@
       <c r="M18" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
+      <c r="N18" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P18" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="S18" s="7">
+        <v>0</v>
+      </c>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
@@ -26536,12 +26764,24 @@
       <c r="M19" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
+      <c r="N19" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P19" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="S19" s="7">
+        <v>0</v>
+      </c>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -26568,12 +26808,24 @@
       <c r="M20" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
+      <c r="N20" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P20" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="S20" s="7">
+        <v>0</v>
+      </c>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
@@ -26600,12 +26852,24 @@
       <c r="M21" s="85" t="s">
         <v>287</v>
       </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
+      <c r="N21" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P21" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0</v>
+      </c>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
@@ -26632,12 +26896,24 @@
       <c r="M22" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="3"/>
+      <c r="N22" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P22" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="S22" s="7">
+        <v>0</v>
+      </c>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
@@ -26664,12 +26940,24 @@
       <c r="M23" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+      <c r="N23" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P23" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="S23" s="7">
+        <v>0</v>
+      </c>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
@@ -26696,12 +26984,24 @@
       <c r="M24" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
+      <c r="N24" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P24" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0</v>
+      </c>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
@@ -26728,12 +27028,24 @@
       <c r="M25" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
+      <c r="N25" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P25" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="S25" s="7">
+        <v>0</v>
+      </c>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -26760,12 +27072,24 @@
       <c r="M26" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
+      <c r="N26" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P26" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="S26" s="7">
+        <v>0</v>
+      </c>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
@@ -26792,12 +27116,24 @@
       <c r="M27" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="N27" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P27" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="S27" s="7">
+        <v>0</v>
+      </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
@@ -26824,12 +27160,24 @@
       <c r="M28" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
+      <c r="N28" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="S28" s="7">
+        <v>0</v>
+      </c>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
@@ -26856,12 +27204,24 @@
       <c r="M29" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
+      <c r="N29" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P29" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="S29" s="7">
+        <v>0</v>
+      </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
@@ -26888,12 +27248,24 @@
       <c r="M30" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
+      <c r="N30" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P30" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="S30" s="7">
+        <v>0</v>
+      </c>
       <c r="T30" s="3"/>
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
@@ -26920,12 +27292,24 @@
       <c r="M31" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
+      <c r="N31" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="S31" s="7">
+        <v>0</v>
+      </c>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
@@ -26952,12 +27336,24 @@
       <c r="M32" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="S32" s="3"/>
+      <c r="N32" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P32" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="S32" s="7">
+        <v>0</v>
+      </c>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
@@ -26984,12 +27380,24 @@
       <c r="M33" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="3"/>
+      <c r="N33" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O33" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R33" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="S33" s="7">
+        <v>0</v>
+      </c>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
@@ -27016,12 +27424,24 @@
       <c r="M34" s="7" t="s">
         <v>298</v>
       </c>
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="S34" s="3"/>
+      <c r="N34" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O34" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P34" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="S34" s="7">
+        <v>0</v>
+      </c>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
@@ -27048,12 +27468,24 @@
       <c r="M35" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
+      <c r="N35" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O35" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P35" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R35" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="S35" s="7">
+        <v>0</v>
+      </c>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
@@ -27080,12 +27512,24 @@
       <c r="M36" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="S36" s="3"/>
+      <c r="N36" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O36" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P36" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0</v>
+      </c>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
@@ -27112,12 +27556,24 @@
       <c r="M37" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="N37" s="3"/>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="S37" s="3"/>
+      <c r="N37" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P37" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R37" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0</v>
+      </c>
       <c r="T37" s="3"/>
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
@@ -27144,12 +27600,24 @@
       <c r="M38" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="3"/>
+      <c r="N38" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P38" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="S38" s="7">
+        <v>0</v>
+      </c>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
@@ -27176,12 +27644,24 @@
       <c r="M39" s="7" t="s">
         <v>464</v>
       </c>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="S39" s="3"/>
+      <c r="N39" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O39" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P39" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="S39" s="7">
+        <v>0</v>
+      </c>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
@@ -27208,12 +27688,24 @@
       <c r="M40" s="7" t="s">
         <v>465</v>
       </c>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="S40" s="3"/>
+      <c r="N40" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P40" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="S40" s="7">
+        <v>0</v>
+      </c>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -27240,12 +27732,24 @@
       <c r="M41" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
+      <c r="N41" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P41" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="S41" s="7">
+        <v>0</v>
+      </c>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
@@ -27272,12 +27776,24 @@
       <c r="M42" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
+      <c r="N42" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P42" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="S42" s="7">
+        <v>0</v>
+      </c>
       <c r="T42" s="3"/>
       <c r="U42" s="3"/>
       <c r="V42" s="3"/>
@@ -27304,12 +27820,24 @@
       <c r="M43" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
+      <c r="N43" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P43" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="S43" s="7">
+        <v>0</v>
+      </c>
       <c r="T43" s="3"/>
       <c r="U43" s="3"/>
       <c r="V43" s="3"/>
@@ -27336,12 +27864,24 @@
       <c r="M44" s="7" t="s">
         <v>469</v>
       </c>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
+      <c r="N44" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P44" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="S44" s="7">
+        <v>0</v>
+      </c>
       <c r="T44" s="3"/>
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
@@ -27380,12 +27920,24 @@
       <c r="M45" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
+      <c r="N45" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O45" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P45" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="S45" s="7">
+        <v>0</v>
+      </c>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
@@ -27412,12 +27964,24 @@
       <c r="M46" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
+      <c r="N46" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O46" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P46" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="S46" s="7">
+        <v>0</v>
+      </c>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
@@ -27444,12 +28008,24 @@
       <c r="M47" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
+      <c r="N47" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O47" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P47" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="S47" s="7">
+        <v>0</v>
+      </c>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
       <c r="V47" s="3"/>
@@ -27488,12 +28064,24 @@
       <c r="M48" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
+      <c r="N48" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O48" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P48" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="S48" s="7">
+        <v>0</v>
+      </c>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
       <c r="V48" s="3"/>
@@ -27520,12 +28108,24 @@
       <c r="M49" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
+      <c r="N49" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O49" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P49" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="S49" s="7">
+        <v>0</v>
+      </c>
       <c r="T49" s="3"/>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
@@ -27552,12 +28152,24 @@
       <c r="M50" s="7" t="s">
         <v>467</v>
       </c>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
+      <c r="N50" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O50" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P50" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="S50" s="7">
+        <v>0</v>
+      </c>
       <c r="T50" s="3"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
@@ -27596,12 +28208,24 @@
       <c r="M51" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
+      <c r="N51" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O51" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P51" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="S51" s="7">
+        <v>0</v>
+      </c>
       <c r="T51" s="3"/>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
@@ -27628,12 +28252,24 @@
       <c r="M52" s="7" t="s">
         <v>483</v>
       </c>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
+      <c r="N52" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O52" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P52" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="S52" s="7">
+        <v>0</v>
+      </c>
       <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
@@ -27672,12 +28308,24 @@
       <c r="M53" s="7" t="s">
         <v>485</v>
       </c>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
+      <c r="N53" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O53" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P53" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R53" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="S53" s="7">
+        <v>0</v>
+      </c>
       <c r="T53" s="3"/>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
@@ -27716,12 +28364,24 @@
       <c r="M54" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
+      <c r="N54" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P54" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="S54" s="7">
+        <v>0</v>
+      </c>
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
@@ -27748,12 +28408,24 @@
       <c r="M55" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
+      <c r="N55" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P55" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R55" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="S55" s="7">
+        <v>0</v>
+      </c>
       <c r="T55" s="3"/>
       <c r="U55" s="3"/>
       <c r="V55" s="3"/>
@@ -27780,12 +28452,24 @@
       <c r="M56" s="7" t="s">
         <v>488</v>
       </c>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
+      <c r="N56" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P56" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="S56" s="7">
+        <v>0</v>
+      </c>
       <c r="T56" s="3"/>
       <c r="U56" s="3"/>
       <c r="V56" s="3"/>
@@ -27824,12 +28508,24 @@
       <c r="M57" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
+      <c r="N57" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P57" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="S57" s="7">
+        <v>0</v>
+      </c>
       <c r="T57" s="3"/>
       <c r="U57" s="3"/>
       <c r="V57" s="3"/>
@@ -27856,12 +28552,24 @@
       <c r="M58" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
+      <c r="N58" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="O58" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="P58" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q58" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>721</v>
+      </c>
+      <c r="S58" s="7">
+        <v>0</v>
+      </c>
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
       <c r="V58" s="3"/>
@@ -27876,7 +28584,7 @@
         <v>9</v>
       </c>
       <c r="M59" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N59" t="s">
         <v>233</v>
@@ -27884,16 +28592,16 @@
       <c r="O59" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P59">
+      <c r="P59" s="7">
         <v>1</v>
       </c>
       <c r="Q59" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R59" s="7" t="s">
-        <v>676</v>
-      </c>
-      <c r="S59">
+        <v>675</v>
+      </c>
+      <c r="S59" s="7">
         <v>0</v>
       </c>
       <c r="T59" s="112" t="s">
@@ -27915,7 +28623,7 @@
         <v>9</v>
       </c>
       <c r="M60" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N60" t="s">
         <v>233</v>
@@ -27923,16 +28631,16 @@
       <c r="O60" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P60">
+      <c r="P60" s="7">
         <v>1</v>
       </c>
       <c r="Q60" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R60" s="7" t="s">
-        <v>631</v>
-      </c>
-      <c r="S60">
+        <v>678</v>
+      </c>
+      <c r="S60" s="7">
         <v>0</v>
       </c>
       <c r="T60" s="112" t="s">
@@ -27953,7 +28661,7 @@
         <v>9</v>
       </c>
       <c r="M61" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N61" t="s">
         <v>233</v>
@@ -27961,16 +28669,16 @@
       <c r="O61" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P61">
+      <c r="P61" s="7">
         <v>1</v>
       </c>
       <c r="Q61" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R61" s="7" t="s">
-        <v>632</v>
-      </c>
-      <c r="S61">
+        <v>631</v>
+      </c>
+      <c r="S61" s="7">
         <v>0</v>
       </c>
       <c r="T61" s="112" t="s">
@@ -27991,7 +28699,7 @@
         <v>9</v>
       </c>
       <c r="M62" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N62" t="s">
         <v>233</v>
@@ -27999,16 +28707,16 @@
       <c r="O62" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P62">
+      <c r="P62" s="7">
         <v>1</v>
       </c>
       <c r="Q62" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R62" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="S62">
+        <v>632</v>
+      </c>
+      <c r="S62" s="7">
         <v>0</v>
       </c>
       <c r="T62" s="112" t="s">
@@ -28029,7 +28737,7 @@
         <v>9</v>
       </c>
       <c r="M63" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N63" t="s">
         <v>233</v>
@@ -28037,16 +28745,16 @@
       <c r="O63" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P63">
+      <c r="P63" s="7">
         <v>1</v>
       </c>
       <c r="Q63" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R63" s="7" t="s">
-        <v>634</v>
-      </c>
-      <c r="S63">
+        <v>633</v>
+      </c>
+      <c r="S63" s="7">
         <v>0</v>
       </c>
       <c r="T63" s="112" t="s">
@@ -28067,7 +28775,7 @@
         <v>9</v>
       </c>
       <c r="M64" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N64" t="s">
         <v>233</v>
@@ -28075,16 +28783,16 @@
       <c r="O64" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P64">
+      <c r="P64" s="7">
         <v>1</v>
       </c>
       <c r="Q64" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R64" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="S64">
+        <v>634</v>
+      </c>
+      <c r="S64" s="7">
         <v>0</v>
       </c>
       <c r="T64" s="112" t="s">
@@ -28105,7 +28813,7 @@
         <v>9</v>
       </c>
       <c r="M65" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N65" t="s">
         <v>233</v>
@@ -28113,16 +28821,16 @@
       <c r="O65" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P65">
+      <c r="P65" s="7">
         <v>1</v>
       </c>
       <c r="Q65" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R65" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="S65">
+        <v>635</v>
+      </c>
+      <c r="S65" s="7">
         <v>0</v>
       </c>
       <c r="T65" s="112" t="s">
@@ -28143,7 +28851,7 @@
         <v>9</v>
       </c>
       <c r="M66" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N66" t="s">
         <v>233</v>
@@ -28151,16 +28859,16 @@
       <c r="O66" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P66">
+      <c r="P66" s="7">
         <v>1</v>
       </c>
       <c r="Q66" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R66" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="S66">
+        <v>636</v>
+      </c>
+      <c r="S66" s="7">
         <v>0</v>
       </c>
       <c r="T66" s="112" t="s">
@@ -28181,7 +28889,7 @@
         <v>9</v>
       </c>
       <c r="M67" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N67" t="s">
         <v>233</v>
@@ -28189,16 +28897,16 @@
       <c r="O67" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P67">
+      <c r="P67" s="7">
         <v>1</v>
       </c>
       <c r="Q67" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R67" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="S67">
+        <v>637</v>
+      </c>
+      <c r="S67" s="7">
         <v>0</v>
       </c>
       <c r="T67" s="112" t="s">
@@ -28219,7 +28927,7 @@
         <v>9</v>
       </c>
       <c r="M68" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N68" t="s">
         <v>233</v>
@@ -28227,16 +28935,16 @@
       <c r="O68" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P68">
+      <c r="P68" s="7">
         <v>1</v>
       </c>
       <c r="Q68" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R68" s="7" t="s">
-        <v>639</v>
-      </c>
-      <c r="S68">
+        <v>638</v>
+      </c>
+      <c r="S68" s="7">
         <v>0</v>
       </c>
       <c r="T68" s="112" t="s">
@@ -28257,7 +28965,7 @@
         <v>9</v>
       </c>
       <c r="M69" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N69" t="s">
         <v>233</v>
@@ -28265,16 +28973,16 @@
       <c r="O69" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P69">
+      <c r="P69" s="7">
         <v>1</v>
       </c>
       <c r="Q69" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R69" s="7" t="s">
-        <v>640</v>
-      </c>
-      <c r="S69">
+        <v>639</v>
+      </c>
+      <c r="S69" s="7">
         <v>0</v>
       </c>
       <c r="T69" s="112" t="s">
@@ -28295,7 +29003,7 @@
         <v>9</v>
       </c>
       <c r="M70" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="N70" t="s">
         <v>233</v>
@@ -28303,16 +29011,16 @@
       <c r="O70" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="P70">
+      <c r="P70" s="7">
         <v>1</v>
       </c>
       <c r="Q70" s="7" t="s">
         <v>273</v>
       </c>
       <c r="R70" s="7" t="s">
-        <v>641</v>
-      </c>
-      <c r="S70">
+        <v>640</v>
+      </c>
+      <c r="S70" s="7">
         <v>0</v>
       </c>
       <c r="T70" s="112" t="s">

</xml_diff>

<commit_message>
Modified test data for Page Validations
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\CodeLessFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881C8BC-8269-4E99-8C9B-538CC8522EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D87480-014B-48B0-B9AD-9481CA1457E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="615" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="615" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5979" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5984" uniqueCount="1139">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -2514,9 +2514,6 @@
     <t>//*[contains(text(),'Field is Required')]</t>
   </si>
   <si>
-    <t>12 3</t>
-  </si>
-  <si>
     <t>//*[contains(text(),'Please Enter Valid AddressLine1')]</t>
   </si>
   <si>
@@ -3448,6 +3445,39 @@
   </si>
   <si>
     <t>AreEqual&gt;Please enter PAN No</t>
+  </si>
+  <si>
+    <t>##&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹1,062 (Premium) + ₹191 (Tax) From the second year onwards ₹1,114 (Premium) +₹201 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹1,895 (Premium) + ₹341 (Tax) From the second year onwards ₹1,993 (Premium) +₹359 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹10,437 (Premium) + ₹1,879 (Tax) From the second year onwards ₹10,950 (Premium) +₹1,971 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹9,999 (Premium) + ₹1,800 (Tax) From the second year onwards ₹10,527 (Premium) +₹1,895 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹5,544 (Premium) + ₹998 (Tax) From the second year onwards ₹5,830 (Premium) +₹1,049 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹597 (Premium) + ₹107 (Tax) From the second year onwards ₹627 (Premium) +₹113 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹967 (Premium) + ₹174 (Tax) From the second year onwards ₹1,019 (Premium) +₹183 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹900 (Premium) + ₹162 (Tax) From the second year onwards ₹948 (Premium) +₹171 (Tax)</t>
+  </si>
+  <si>
+    <t>AreEqual&gt;For First Year ₹14,840 (Premium) + ₹2,671 (Tax) From the second year onwards ₹15,615 (Premium) +₹2,811 (Tax)</t>
+  </si>
+  <si>
+    <t>//*[@id="personalDetailsForm"]/section/div/button[2]</t>
   </si>
 </sst>
 </file>
@@ -3457,7 +3487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3533,6 +3563,12 @@
       <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3876,7 +3912,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4485,6 +4521,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5184,8 +5223,8 @@
   <dimension ref="A1:V147"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M142" sqref="M142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7648,7 +7687,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="61" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>35</v>
@@ -7689,7 +7728,7 @@
         <v>1</v>
       </c>
       <c r="C64" s="61" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D64" s="38" t="s">
         <v>35</v>
@@ -7728,7 +7767,7 @@
         <v>1</v>
       </c>
       <c r="C65" s="61" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="38" t="s">
@@ -7767,7 +7806,7 @@
         <v>1</v>
       </c>
       <c r="C66" s="61" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D66" s="38" t="s">
         <v>35</v>
@@ -7806,7 +7845,7 @@
         <v>1</v>
       </c>
       <c r="C67" s="61" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>35</v>
@@ -7845,7 +7884,7 @@
         <v>1</v>
       </c>
       <c r="C68" s="61" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D68" s="38" t="s">
         <v>35</v>
@@ -7884,7 +7923,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="61" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="38" t="s">
@@ -7923,7 +7962,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="61" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>35</v>
@@ -7962,7 +8001,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="61" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="38" t="s">
@@ -8001,7 +8040,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="61" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>35</v>
@@ -8042,7 +8081,7 @@
         <v>1</v>
       </c>
       <c r="C73" s="61" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D73" s="38" t="s">
         <v>35</v>
@@ -8083,7 +8122,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="61" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="38" t="s">
@@ -8124,7 +8163,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="61" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D75" s="38" t="s">
         <v>35</v>
@@ -8163,7 +8202,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="61" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="38" t="s">
@@ -8204,7 +8243,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="61" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D77" s="38" t="s">
         <v>35</v>
@@ -8245,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="61" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="38" t="s">
@@ -8288,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="61" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D79" s="38" t="s">
         <v>35</v>
@@ -8331,7 +8370,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="61" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="38" t="s">
@@ -8372,7 +8411,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="61" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D81" s="38" t="s">
         <v>35</v>
@@ -8413,7 +8452,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="61" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="D82" s="38" t="s">
         <v>35</v>
@@ -8452,7 +8491,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="61" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="38" t="s">
@@ -8491,7 +8530,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="61" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D84" s="38" t="s">
         <v>35</v>
@@ -8530,7 +8569,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="61" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D85" s="38" t="s">
         <v>35</v>
@@ -8569,7 +8608,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="61" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D86" s="169"/>
       <c r="E86" s="196" t="s">
@@ -9922,7 +9961,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="143" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D124" s="143"/>
       <c r="E124" s="143"/>
@@ -9955,7 +9994,7 @@
         <v>2</v>
       </c>
       <c r="C125" s="143" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D125" s="143" t="s">
         <v>35</v>
@@ -9989,7 +10028,7 @@
         <v>3</v>
       </c>
       <c r="C126" s="143" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D126" s="143"/>
       <c r="E126" s="143"/>
@@ -10023,7 +10062,7 @@
         <v>4</v>
       </c>
       <c r="C127" s="143" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D127" s="143"/>
       <c r="E127" s="143"/>
@@ -10057,7 +10096,7 @@
         <v>5</v>
       </c>
       <c r="C128" s="143" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D128" s="143"/>
       <c r="E128" s="143"/>
@@ -10090,7 +10129,7 @@
         <v>6</v>
       </c>
       <c r="C129" s="143" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D129" s="143"/>
       <c r="E129" s="143"/>
@@ -10123,7 +10162,7 @@
         <v>7</v>
       </c>
       <c r="C130" s="143" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D130" s="143"/>
       <c r="E130" s="143"/>
@@ -10156,7 +10195,7 @@
         <v>8</v>
       </c>
       <c r="C131" s="143" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D131" s="143"/>
       <c r="E131" s="143"/>
@@ -10189,7 +10228,7 @@
         <v>9</v>
       </c>
       <c r="C132" s="143" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D132" s="143"/>
       <c r="E132" s="143"/>
@@ -10222,7 +10261,7 @@
         <v>10</v>
       </c>
       <c r="C133" s="143" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D133" s="143"/>
       <c r="E133" s="143"/>
@@ -10255,7 +10294,7 @@
         <v>11</v>
       </c>
       <c r="C134" s="143" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D134" s="143"/>
       <c r="E134" s="143"/>
@@ -10287,7 +10326,7 @@
         <v>12</v>
       </c>
       <c r="C135" s="143" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D135" s="143"/>
       <c r="E135" s="143"/>
@@ -10319,7 +10358,7 @@
         <v>13</v>
       </c>
       <c r="C136" s="143" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D136" s="143"/>
       <c r="E136" s="143"/>
@@ -10351,7 +10390,7 @@
         <v>14</v>
       </c>
       <c r="C137" s="143" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D137" s="143"/>
       <c r="E137" s="143"/>
@@ -10488,7 +10527,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="143" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D141" s="193" t="s">
         <v>35</v>
@@ -10524,7 +10563,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="143" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D142" s="193" t="s">
         <v>35</v>
@@ -10560,7 +10599,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="143" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D143" s="193" t="s">
         <v>35</v>
@@ -10571,7 +10610,7 @@
         <v>35</v>
       </c>
       <c r="H143" s="194" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="I143" s="143"/>
       <c r="J143" s="143"/>
@@ -10596,7 +10635,7 @@
         <v>1</v>
       </c>
       <c r="C144" s="143" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D144" s="193" t="s">
         <v>35</v>
@@ -10632,7 +10671,7 @@
         <v>1</v>
       </c>
       <c r="C145" s="143" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D145" s="193" t="s">
         <v>35</v>
@@ -10643,7 +10682,7 @@
         <v>35</v>
       </c>
       <c r="H145" s="194" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="I145" s="143"/>
       <c r="J145" s="143"/>
@@ -10668,7 +10707,7 @@
         <v>1</v>
       </c>
       <c r="C146" s="143" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D146" s="193" t="s">
         <v>35</v>
@@ -10679,7 +10718,7 @@
         <v>35</v>
       </c>
       <c r="H146" s="194" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="I146" s="143"/>
       <c r="J146" s="143"/>
@@ -10704,7 +10743,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="143" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D147" s="193" t="s">
         <v>35</v>
@@ -10715,7 +10754,7 @@
         <v>35</v>
       </c>
       <c r="H147" s="194" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="I147" s="143"/>
       <c r="J147" s="143"/>
@@ -10761,8 +10800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10786,7 +10825,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="93" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D1" s="93" t="s">
         <v>316</v>
@@ -10804,10 +10843,10 @@
         <v>320</v>
       </c>
       <c r="I1" s="93" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="J1" s="93" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -10837,7 +10876,7 @@
         <v>816</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -11319,10 +11358,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>817</v>
+        <v>1128</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -11355,10 +11394,10 @@
         <v>10</v>
       </c>
       <c r="C25" s="132" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>1025</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>1026</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
@@ -11377,10 +11416,10 @@
         <v>10</v>
       </c>
       <c r="C26" s="132" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>1027</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>1028</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
@@ -11399,10 +11438,10 @@
         <v>10</v>
       </c>
       <c r="C27" s="132" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>1029</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>1030</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
@@ -11421,10 +11460,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="132" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>1031</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>1032</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
@@ -11443,10 +11482,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="132" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>1033</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>1034</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
@@ -11468,9 +11507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5832304-EC06-40FE-8487-FD1C740F42DA}">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W29" sqref="W29"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB32" sqref="AB29:AB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11486,9 +11525,11 @@
     <col min="11" max="12" width="19" customWidth="1"/>
     <col min="13" max="14" width="15.85546875" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" customWidth="1"/>
-    <col min="16" max="22" width="10.85546875" customWidth="1"/>
-    <col min="23" max="23" width="15" customWidth="1"/>
-    <col min="24" max="27" width="16.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" customWidth="1"/>
+    <col min="17" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="25" width="10.85546875" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" customWidth="1"/>
     <col min="28" max="28" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11512,10 +11553,10 @@
         <v>323</v>
       </c>
       <c r="G1" s="149" t="s">
+        <v>842</v>
+      </c>
+      <c r="H1" s="149" t="s">
         <v>843</v>
-      </c>
-      <c r="H1" s="149" t="s">
-        <v>844</v>
       </c>
       <c r="I1" s="149" t="s">
         <v>324</v>
@@ -11533,7 +11574,7 @@
         <v>328</v>
       </c>
       <c r="N1" s="149" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="O1" s="149" t="s">
         <v>329</v>
@@ -11542,37 +11583,37 @@
         <v>330</v>
       </c>
       <c r="Q1" s="149" t="s">
+        <v>856</v>
+      </c>
+      <c r="R1" s="149" t="s">
+        <v>857</v>
+      </c>
+      <c r="S1" s="149" t="s">
+        <v>855</v>
+      </c>
+      <c r="T1" s="149" t="s">
+        <v>830</v>
+      </c>
+      <c r="U1" s="149" t="s">
         <v>831</v>
       </c>
-      <c r="R1" s="149" t="s">
+      <c r="V1" s="149" t="s">
         <v>832</v>
       </c>
-      <c r="S1" s="149" t="s">
+      <c r="W1" s="149" t="s">
         <v>833</v>
       </c>
-      <c r="T1" s="149" t="s">
+      <c r="X1" s="149" t="s">
         <v>834</v>
       </c>
-      <c r="U1" s="149" t="s">
+      <c r="Y1" s="149" t="s">
         <v>835</v>
       </c>
-      <c r="V1" s="149" t="s">
-        <v>836</v>
-      </c>
-      <c r="W1" s="149" t="s">
-        <v>821</v>
-      </c>
-      <c r="X1" s="149" t="s">
-        <v>823</v>
-      </c>
-      <c r="Y1" s="149" t="s">
-        <v>857</v>
-      </c>
       <c r="Z1" s="149" t="s">
-        <v>858</v>
+        <v>820</v>
       </c>
       <c r="AA1" s="149" t="s">
-        <v>856</v>
+        <v>822</v>
       </c>
       <c r="AB1" s="149" t="s">
         <v>331</v>
@@ -11596,10 +11637,10 @@
         <v>339</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>844</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>845</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>846</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>340</v>
@@ -11617,46 +11658,46 @@
         <v>344</v>
       </c>
       <c r="N2" s="15" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="O2" s="15" t="s">
         <v>345</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>853</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>858</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>827</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>829</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>830</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>824</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>820</v>
-      </c>
-      <c r="Y2" s="15" t="s">
-        <v>854</v>
-      </c>
       <c r="Z2" s="15" t="s">
-        <v>859</v>
+        <v>823</v>
       </c>
       <c r="AA2" s="15" t="s">
-        <v>789</v>
+        <v>819</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>346</v>
@@ -11677,7 +11718,9 @@
         <v>5000</v>
       </c>
       <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>30</v>
+      </c>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
@@ -11687,15 +11730,17 @@
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="3" t="s">
+        <v>420</v>
+      </c>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="15"/>
       <c r="AB3" s="7" t="s">
@@ -11745,15 +11790,15 @@
       <c r="P4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="15"/>
       <c r="AB4" s="7" t="s">
@@ -11803,15 +11848,15 @@
       <c r="P5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
       <c r="AA5" s="15"/>
       <c r="AB5" s="7" t="s">
@@ -11861,15 +11906,15 @@
       <c r="P6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
       <c r="AA6" s="15"/>
       <c r="AB6" s="7" t="s">
@@ -11919,15 +11964,15 @@
       <c r="P7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
       <c r="AA7" s="15"/>
       <c r="AB7" s="3"/>
@@ -11975,15 +12020,15 @@
       <c r="P8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
       <c r="AA8" s="15"/>
       <c r="AB8" s="7" t="s">
@@ -12033,15 +12078,15 @@
       <c r="P9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
       <c r="Z9" s="15"/>
       <c r="AA9" s="15"/>
       <c r="AB9" s="7" t="s">
@@ -12091,15 +12136,15 @@
       <c r="P10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
       <c r="Z10" s="15"/>
       <c r="AA10" s="15"/>
       <c r="AB10" s="7" t="s">
@@ -12149,15 +12194,15 @@
       <c r="P11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
       <c r="Z11" s="15"/>
       <c r="AA11" s="15"/>
       <c r="AB11" s="7" t="s">
@@ -12207,15 +12252,15 @@
       <c r="P12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
       <c r="Z12" s="15"/>
       <c r="AA12" s="15"/>
       <c r="AB12" s="7" t="s">
@@ -12265,15 +12310,15 @@
       <c r="P13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
-      <c r="W13" s="15"/>
-      <c r="X13" s="15"/>
-      <c r="Y13" s="15"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="15"/>
       <c r="AB13" s="7" t="s">
@@ -12323,15 +12368,15 @@
       <c r="P14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
       <c r="Z14" s="15"/>
       <c r="AA14" s="15"/>
       <c r="AB14" s="7" t="s">
@@ -12381,15 +12426,15 @@
       <c r="P15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
       <c r="AA15" s="15"/>
       <c r="AB15" s="7" t="s">
@@ -12439,15 +12484,15 @@
       <c r="P16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
       <c r="Z16" s="15"/>
       <c r="AA16" s="15"/>
       <c r="AB16" s="7" t="s">
@@ -12497,15 +12542,15 @@
       <c r="P17" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
       <c r="Z17" s="15"/>
       <c r="AA17" s="15"/>
       <c r="AB17" s="7" t="s">
@@ -12555,15 +12600,15 @@
       <c r="P18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
       <c r="Z18" s="15"/>
       <c r="AA18" s="15"/>
       <c r="AB18" s="7" t="s">
@@ -12613,15 +12658,15 @@
       <c r="P19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
       <c r="Z19" s="15"/>
       <c r="AA19" s="15"/>
       <c r="AB19" s="7" t="s">
@@ -12671,15 +12716,15 @@
       <c r="P20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
       <c r="Z20" s="15"/>
       <c r="AA20" s="15"/>
       <c r="AB20" s="7" t="s">
@@ -12729,9 +12774,9 @@
       <c r="P21" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
       <c r="AA21" s="15"/>
       <c r="AB21" s="7" t="s">
         <v>35</v>
@@ -12748,33 +12793,33 @@
       <c r="P22" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>837</v>
       </c>
-      <c r="R22" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="W22" s="2" t="s">
         <v>839</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="X22" s="2" t="s">
         <v>840</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="Y22" s="2" t="s">
         <v>841</v>
       </c>
-      <c r="V22" s="2" t="s">
-        <v>842</v>
-      </c>
-      <c r="W22" s="1">
+      <c r="Z22" s="1">
         <v>12345678910</v>
       </c>
-      <c r="X22" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
+      <c r="AA22" s="2" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
@@ -12796,9 +12841,9 @@
         <v>25</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>847</v>
-      </c>
-      <c r="W23" s="1"/>
+        <v>846</v>
+      </c>
+      <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="24">
@@ -12811,7 +12856,7 @@
         <v>250</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -12840,7 +12885,10 @@
         <v>123</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
+      </c>
+      <c r="Z25">
+        <v>889857669522</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -12851,20 +12899,21 @@
         <v>15</v>
       </c>
       <c r="M26" t="s">
+        <v>851</v>
+      </c>
+      <c r="O26" t="s">
         <v>852</v>
       </c>
-      <c r="O26" t="s">
-        <v>853</v>
-      </c>
       <c r="P26" t="s">
         <v>35</v>
       </c>
-      <c r="Y26" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>35</v>
-      </c>
+      <c r="Q26" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="S26" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB26" s="2"/>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="24">
@@ -12874,20 +12923,21 @@
         <v>16</v>
       </c>
       <c r="M27" t="s">
+        <v>860</v>
+      </c>
+      <c r="O27" t="s">
         <v>861</v>
       </c>
-      <c r="O27" t="s">
-        <v>862</v>
-      </c>
       <c r="P27" t="s">
         <v>35</v>
       </c>
-      <c r="Z27" s="26" t="s">
-        <v>860</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>35</v>
-      </c>
+      <c r="R27" s="26" t="s">
+        <v>859</v>
+      </c>
+      <c r="S27" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB27" s="2"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="24">
@@ -12932,9 +12982,9 @@
       <c r="P28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X28" s="178"/>
-      <c r="Y28" s="178"/>
-      <c r="Z28" s="178"/>
+      <c r="Q28" s="178"/>
+      <c r="R28" s="178"/>
+      <c r="S28" s="178"/>
       <c r="AA28" s="178"/>
       <c r="AB28" s="2" t="s">
         <v>35</v>
@@ -12983,9 +13033,9 @@
       <c r="P29" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X29" s="178"/>
-      <c r="Y29" s="178"/>
-      <c r="Z29" s="178"/>
+      <c r="Q29" s="178"/>
+      <c r="R29" s="178"/>
+      <c r="S29" s="178"/>
       <c r="AA29" s="178"/>
       <c r="AB29" s="2" t="s">
         <v>35</v>
@@ -13034,9 +13084,9 @@
       <c r="P30" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X30" s="178"/>
-      <c r="Y30" s="178"/>
-      <c r="Z30" s="178"/>
+      <c r="Q30" s="178"/>
+      <c r="R30" s="178"/>
+      <c r="S30" s="178"/>
       <c r="AA30" s="178"/>
       <c r="AB30" s="2" t="s">
         <v>35</v>
@@ -13085,9 +13135,9 @@
       <c r="P31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X31" s="178"/>
-      <c r="Y31" s="178"/>
-      <c r="Z31" s="178"/>
+      <c r="Q31" s="178"/>
+      <c r="R31" s="178"/>
+      <c r="S31" s="178"/>
       <c r="AA31" s="178"/>
       <c r="AB31" s="2" t="s">
         <v>35</v>
@@ -13136,9 +13186,9 @@
       <c r="P32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X32" s="178"/>
-      <c r="Y32" s="178"/>
-      <c r="Z32" s="178"/>
+      <c r="Q32" s="178"/>
+      <c r="R32" s="178"/>
+      <c r="S32" s="178"/>
       <c r="AA32" s="178"/>
       <c r="AB32" s="2" t="s">
         <v>35</v>
@@ -13154,8 +13204,8 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13194,7 +13244,7 @@
         <v>368</v>
       </c>
       <c r="F1" s="182" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="G1" s="182" t="s">
         <v>369</v>
@@ -13206,16 +13256,16 @@
         <v>371</v>
       </c>
       <c r="J1" s="153" t="s">
+        <v>865</v>
+      </c>
+      <c r="K1" s="153" t="s">
         <v>866</v>
       </c>
-      <c r="K1" s="153" t="s">
+      <c r="L1" s="153" t="s">
         <v>867</v>
       </c>
-      <c r="L1" s="153" t="s">
+      <c r="M1" s="153" t="s">
         <v>868</v>
-      </c>
-      <c r="M1" s="153" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -13233,7 +13283,7 @@
         <v>396</v>
       </c>
       <c r="F2" s="143" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="G2" s="143" t="s">
         <v>397</v>
@@ -13245,16 +13295,16 @@
         <v>399</v>
       </c>
       <c r="J2" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="K2" t="s">
+        <v>869</v>
+      </c>
+      <c r="L2" t="s">
         <v>870</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>871</v>
-      </c>
-      <c r="M2" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -13624,16 +13674,16 @@
         <v>35</v>
       </c>
       <c r="J22" s="167" t="s">
+        <v>872</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>875</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -13650,7 +13700,7 @@
         <v>22222015</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="I23" s="143"/>
     </row>
@@ -13790,31 +13840,31 @@
         <v>379</v>
       </c>
       <c r="K1" s="152" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="L1" s="152" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="M1" s="152" t="s">
         <v>380</v>
       </c>
       <c r="N1" s="152" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="O1" s="185" t="s">
         <v>764</v>
       </c>
       <c r="P1" s="187" t="s">
+        <v>894</v>
+      </c>
+      <c r="Q1" s="188" t="s">
+        <v>891</v>
+      </c>
+      <c r="R1" s="188" t="s">
+        <v>892</v>
+      </c>
+      <c r="S1" s="188" t="s">
         <v>895</v>
-      </c>
-      <c r="Q1" s="188" t="s">
-        <v>892</v>
-      </c>
-      <c r="R1" s="188" t="s">
-        <v>893</v>
-      </c>
-      <c r="S1" s="188" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -13847,31 +13897,31 @@
         <v>406</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>407</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>789</v>
       </c>
       <c r="P2" s="186" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="Q2" s="186" t="s">
+        <v>885</v>
+      </c>
+      <c r="R2" s="186" t="s">
         <v>886</v>
       </c>
-      <c r="R2" s="186" t="s">
+      <c r="S2" s="186" t="s">
         <v>887</v>
-      </c>
-      <c r="S2" s="186" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -14453,7 +14503,7 @@
         <v>35</v>
       </c>
       <c r="N22" s="189" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="O22" s="6" t="s">
         <v>35</v>
@@ -14483,13 +14533,13 @@
         <v>35</v>
       </c>
       <c r="Q23" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="R23" s="2" t="s">
         <v>889</v>
       </c>
-      <c r="R23" s="2" t="s">
+      <c r="S23" s="2" t="s">
         <v>890</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -14596,160 +14646,160 @@
         <v>1</v>
       </c>
       <c r="C1" s="113" t="s">
+        <v>897</v>
+      </c>
+      <c r="D1" s="113" t="s">
         <v>898</v>
       </c>
-      <c r="D1" s="113" t="s">
-        <v>899</v>
-      </c>
       <c r="E1" s="113" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F1" s="113" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G1" s="113" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H1" s="113" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="I1" s="113" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="J1" s="113" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="K1" s="113" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="L1" s="113" t="s">
+        <v>918</v>
+      </c>
+      <c r="M1" s="113" t="s">
         <v>919</v>
       </c>
-      <c r="M1" s="113" t="s">
+      <c r="N1" s="141" t="s">
         <v>920</v>
       </c>
-      <c r="N1" s="141" t="s">
-        <v>921</v>
-      </c>
       <c r="O1" s="141" t="s">
+        <v>922</v>
+      </c>
+      <c r="P1" s="141" t="s">
         <v>923</v>
       </c>
-      <c r="P1" s="141" t="s">
-        <v>924</v>
-      </c>
       <c r="Q1" s="141" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="R1" s="141" t="s">
+        <v>935</v>
+      </c>
+      <c r="S1" s="141" t="s">
+        <v>930</v>
+      </c>
+      <c r="T1" s="141" t="s">
+        <v>932</v>
+      </c>
+      <c r="U1" s="141" t="s">
+        <v>926</v>
+      </c>
+      <c r="V1" s="141" t="s">
         <v>936</v>
       </c>
-      <c r="S1" s="141" t="s">
-        <v>931</v>
-      </c>
-      <c r="T1" s="141" t="s">
-        <v>933</v>
-      </c>
-      <c r="U1" s="141" t="s">
-        <v>927</v>
-      </c>
-      <c r="V1" s="141" t="s">
+      <c r="W1" s="141" t="s">
         <v>937</v>
       </c>
-      <c r="W1" s="141" t="s">
-        <v>938</v>
-      </c>
       <c r="X1" s="141" t="s">
+        <v>939</v>
+      </c>
+      <c r="Y1" s="141" t="s">
         <v>940</v>
       </c>
-      <c r="Y1" s="141" t="s">
+      <c r="Z1" s="141" t="s">
         <v>941</v>
       </c>
-      <c r="Z1" s="141" t="s">
-        <v>942</v>
-      </c>
       <c r="AA1" s="141" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="AB1" s="141" t="s">
+        <v>945</v>
+      </c>
+      <c r="AC1" s="141" t="s">
         <v>946</v>
       </c>
-      <c r="AC1" s="141" t="s">
+      <c r="AD1" s="141" t="s">
         <v>947</v>
       </c>
-      <c r="AD1" s="141" t="s">
+      <c r="AE1" s="141" t="s">
         <v>948</v>
       </c>
-      <c r="AE1" s="141" t="s">
-        <v>949</v>
-      </c>
       <c r="AF1" s="141" t="s">
+        <v>950</v>
+      </c>
+      <c r="AG1" s="141" t="s">
         <v>951</v>
       </c>
-      <c r="AG1" s="141" t="s">
+      <c r="AH1" s="141" t="s">
         <v>952</v>
       </c>
-      <c r="AH1" s="141" t="s">
+      <c r="AI1" s="141" t="s">
         <v>953</v>
       </c>
-      <c r="AI1" s="141" t="s">
+      <c r="AJ1" s="141" t="s">
         <v>954</v>
       </c>
-      <c r="AJ1" s="141" t="s">
+      <c r="AK1" s="141" t="s">
         <v>955</v>
       </c>
-      <c r="AK1" s="141" t="s">
+      <c r="AL1" s="141" t="s">
         <v>956</v>
       </c>
-      <c r="AL1" s="141" t="s">
-        <v>957</v>
-      </c>
       <c r="AM1" s="141" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="AN1" s="141" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="AO1" s="141" t="s">
+        <v>963</v>
+      </c>
+      <c r="AP1" s="141" t="s">
         <v>964</v>
       </c>
-      <c r="AP1" s="141" t="s">
-        <v>965</v>
-      </c>
       <c r="AQ1" s="141" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="AR1" s="141" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="AS1" s="141" t="s">
+        <v>971</v>
+      </c>
+      <c r="AT1" s="141" t="s">
         <v>972</v>
       </c>
-      <c r="AT1" s="141" t="s">
-        <v>973</v>
-      </c>
       <c r="AU1" s="141" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="AV1" s="141" t="s">
+        <v>976</v>
+      </c>
+      <c r="AW1" s="141" t="s">
         <v>977</v>
       </c>
-      <c r="AW1" s="141" t="s">
-        <v>978</v>
-      </c>
       <c r="AX1" s="141" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="AY1" s="141" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="AZ1" s="141" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="BA1" s="141" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="BB1" s="141" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="BC1" s="152" t="s">
         <v>381</v>
@@ -14770,160 +14820,160 @@
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>905</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>906</v>
-      </c>
       <c r="I2" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="L2" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>915</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>916</v>
-      </c>
       <c r="N2" s="7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="P2" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>925</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>926</v>
-      </c>
       <c r="R2" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="S2" s="7" t="s">
         <v>929</v>
       </c>
-      <c r="S2" s="7" t="s">
-        <v>930</v>
-      </c>
       <c r="T2" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AB2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="AF2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AH2" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AI2" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="AJ2" s="7" t="s">
         <v>162</v>
       </c>
       <c r="AK2" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AM2" s="7" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="AN2" s="7" t="s">
         <v>170</v>
       </c>
       <c r="AO2" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="AP2" s="7" t="s">
         <v>962</v>
       </c>
-      <c r="AP2" s="7" t="s">
-        <v>963</v>
-      </c>
       <c r="AQ2" s="7" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="AR2" s="7" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="AS2" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AT2" s="7" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="AU2" s="7" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="AV2" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="AW2" s="7" t="s">
         <v>979</v>
       </c>
-      <c r="AW2" s="7" t="s">
-        <v>980</v>
-      </c>
       <c r="AX2" s="7" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="AY2" s="7" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="AZ2" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="BA2" s="7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="BB2" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="BC2" s="3" t="s">
         <v>408</v>
@@ -16238,7 +16288,7 @@
         <v>35</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F22" s="143" t="s">
         <v>35</v>
@@ -16250,7 +16300,7 @@
         <v>35</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>35</v>
@@ -16259,11 +16309,11 @@
         <v>35</v>
       </c>
       <c r="L22" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="M22" s="2" t="s">
         <v>917</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>918</v>
-      </c>
       <c r="N22" s="131" t="s">
         <v>35</v>
       </c>
@@ -16274,7 +16324,7 @@
         <v>35</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>35</v>
@@ -16286,7 +16336,7 @@
         <v>12345</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="V22" s="2" t="s">
         <v>35</v>
@@ -16298,7 +16348,7 @@
         <v>35</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="Z22" s="2" t="s">
         <v>35</v>
@@ -16310,7 +16360,7 @@
         <v>35</v>
       </c>
       <c r="AC22" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AD22" s="2" t="s">
         <v>35</v>
@@ -16322,7 +16372,7 @@
         <v>35</v>
       </c>
       <c r="AG22" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AH22" s="2" t="s">
         <v>35</v>
@@ -16334,7 +16384,7 @@
         <v>35</v>
       </c>
       <c r="AK22" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="AL22" s="2" t="s">
         <v>35</v>
@@ -16346,10 +16396,10 @@
         <v>35</v>
       </c>
       <c r="AO22" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="AP22" s="2" t="s">
         <v>966</v>
-      </c>
-      <c r="AP22" s="2" t="s">
-        <v>967</v>
       </c>
       <c r="AQ22" s="2">
         <v>123</v>
@@ -16367,22 +16417,22 @@
         <v>35</v>
       </c>
       <c r="AV22" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="AW22" s="2" t="s">
         <v>981</v>
-      </c>
-      <c r="AW22" s="2" t="s">
-        <v>982</v>
       </c>
       <c r="AX22" s="2">
         <v>123456789123</v>
       </c>
       <c r="AY22" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="AZ22" s="2">
         <v>254438486541</v>
       </c>
       <c r="BA22" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="BB22" s="2" t="s">
         <v>35</v>
@@ -16428,7 +16478,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16500,10 +16550,10 @@
         <v>393</v>
       </c>
       <c r="Q1" s="153" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="R1" s="153" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -16546,7 +16596,7 @@
         <v>419</v>
       </c>
       <c r="Q2" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="R2" t="s">
         <v>789</v>
@@ -17144,6 +17194,9 @@
       <c r="B17" s="7">
         <v>15</v>
       </c>
+      <c r="C17" t="s">
+        <v>224</v>
+      </c>
       <c r="D17" s="95" t="s">
         <v>224</v>
       </c>
@@ -17332,6 +17385,9 @@
       <c r="B21" s="16">
         <v>15</v>
       </c>
+      <c r="C21" t="s">
+        <v>224</v>
+      </c>
       <c r="D21" s="95" t="s">
         <v>224</v>
       </c>
@@ -17383,7 +17439,7 @@
         <v>35</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="R22" t="s">
         <v>35</v>
@@ -17473,25 +17529,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="192" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1" s="192" t="s">
         <v>997</v>
       </c>
-      <c r="D1" s="192" t="s">
+      <c r="E1" s="192" t="s">
         <v>998</v>
       </c>
-      <c r="E1" s="192" t="s">
+      <c r="F1" s="192" t="s">
         <v>999</v>
       </c>
-      <c r="F1" s="192" t="s">
+      <c r="G1" s="192" t="s">
         <v>1000</v>
       </c>
-      <c r="G1" s="192" t="s">
+      <c r="H1" s="192" t="s">
         <v>1001</v>
       </c>
-      <c r="H1" s="192" t="s">
+      <c r="I1" s="192" t="s">
         <v>1002</v>
-      </c>
-      <c r="I1" s="192" t="s">
-        <v>1003</v>
       </c>
       <c r="J1" s="192" t="s">
         <v>421</v>
@@ -18273,22 +18329,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="150" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D1" s="150" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E1" s="150" t="s">
         <v>766</v>
       </c>
       <c r="F1" s="150" t="s">
+        <v>1010</v>
+      </c>
+      <c r="G1" s="150" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H1" s="150" t="s">
         <v>1011</v>
-      </c>
-      <c r="G1" s="150" t="s">
-        <v>1016</v>
-      </c>
-      <c r="H1" s="150" t="s">
-        <v>1012</v>
       </c>
       <c r="I1" s="150" t="s">
         <v>766</v>
@@ -18303,22 +18359,22 @@
         <v>309</v>
       </c>
       <c r="D2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H2" t="s">
         <v>1009</v>
       </c>
-      <c r="G2" t="s">
-        <v>1014</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1010</v>
-      </c>
       <c r="I2" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -18338,22 +18394,22 @@
         <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F4" s="104" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="H4" s="157" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
   </sheetData>
@@ -18672,7 +18728,7 @@
         <v>679</v>
       </c>
       <c r="I5" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J5">
         <v>25000</v>
@@ -18696,13 +18752,13 @@
         <v>25</v>
       </c>
       <c r="Q5" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R5" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S5" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T5">
         <v>40</v>
@@ -18714,7 +18770,7 @@
         <v>686</v>
       </c>
       <c r="W5" s="122" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="X5" s="122" t="s">
         <v>688</v>
@@ -18755,7 +18811,7 @@
         <v>679</v>
       </c>
       <c r="I6" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J6">
         <v>25000</v>
@@ -18779,13 +18835,13 @@
         <v>25</v>
       </c>
       <c r="Q6" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R6" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S6" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T6">
         <v>40</v>
@@ -18797,7 +18853,7 @@
         <v>686</v>
       </c>
       <c r="W6" s="122" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="X6" s="122" t="s">
         <v>688</v>
@@ -18862,7 +18918,7 @@
         <v>25</v>
       </c>
       <c r="Q7" s="122" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R7" s="122" t="s">
         <v>683</v>
@@ -18880,7 +18936,7 @@
         <v>686</v>
       </c>
       <c r="W7" s="122" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="X7" s="122" t="s">
         <v>688</v>
@@ -18921,7 +18977,7 @@
         <v>679</v>
       </c>
       <c r="I8" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J8">
         <v>25000</v>
@@ -18951,7 +19007,7 @@
         <v>131</v>
       </c>
       <c r="S8" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T8">
         <v>40</v>
@@ -18963,7 +19019,7 @@
         <v>686</v>
       </c>
       <c r="W8" s="122" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="X8" s="122" t="s">
         <v>688</v>
@@ -19004,7 +19060,7 @@
         <v>679</v>
       </c>
       <c r="I9" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J9">
         <v>25000</v>
@@ -19028,13 +19084,13 @@
         <v>25</v>
       </c>
       <c r="Q9" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R9" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S9" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T9">
         <v>40</v>
@@ -19046,7 +19102,7 @@
         <v>686</v>
       </c>
       <c r="W9" s="122" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="X9" s="122" t="s">
         <v>688</v>
@@ -19111,7 +19167,7 @@
         <v>25</v>
       </c>
       <c r="Q10" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R10" s="122" t="s">
         <v>683</v>
@@ -19129,7 +19185,7 @@
         <v>686</v>
       </c>
       <c r="W10" s="122" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="X10" s="122" t="s">
         <v>688</v>
@@ -19170,7 +19226,7 @@
         <v>679</v>
       </c>
       <c r="I11" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J11">
         <v>25000</v>
@@ -19194,13 +19250,13 @@
         <v>25</v>
       </c>
       <c r="Q11" s="122" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R11" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S11" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T11">
         <v>40</v>
@@ -19212,7 +19268,7 @@
         <v>686</v>
       </c>
       <c r="W11" s="122" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="X11" s="122" t="s">
         <v>688</v>
@@ -19253,7 +19309,7 @@
         <v>679</v>
       </c>
       <c r="I12" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J12">
         <v>25000</v>
@@ -19280,10 +19336,10 @@
         <v>682</v>
       </c>
       <c r="R12" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S12" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T12">
         <v>40</v>
@@ -19295,7 +19351,7 @@
         <v>686</v>
       </c>
       <c r="W12" s="122" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="X12" s="122" t="s">
         <v>688</v>
@@ -19360,7 +19416,7 @@
         <v>25</v>
       </c>
       <c r="Q13" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R13" s="122" t="s">
         <v>683</v>
@@ -19378,7 +19434,7 @@
         <v>686</v>
       </c>
       <c r="W13" s="122" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="X13" s="122" t="s">
         <v>688</v>
@@ -19419,7 +19475,7 @@
         <v>679</v>
       </c>
       <c r="I14" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J14">
         <v>25000</v>
@@ -19443,13 +19499,13 @@
         <v>25</v>
       </c>
       <c r="Q14" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R14" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S14" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T14">
         <v>40</v>
@@ -19461,7 +19517,7 @@
         <v>686</v>
       </c>
       <c r="W14" s="122" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="X14" s="122" t="s">
         <v>688</v>
@@ -19502,7 +19558,7 @@
         <v>679</v>
       </c>
       <c r="I15" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J15">
         <v>25000</v>
@@ -19526,13 +19582,13 @@
         <v>25</v>
       </c>
       <c r="Q15" s="122" t="s">
+        <v>1113</v>
+      </c>
+      <c r="R15" s="122" t="s">
         <v>1114</v>
       </c>
-      <c r="R15" s="122" t="s">
-        <v>1115</v>
-      </c>
       <c r="S15" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T15">
         <v>40</v>
@@ -19544,7 +19600,7 @@
         <v>686</v>
       </c>
       <c r="W15" s="122" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="X15" s="122" t="s">
         <v>688</v>
@@ -19627,7 +19683,7 @@
         <v>686</v>
       </c>
       <c r="W16" s="122" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="X16" s="122" t="s">
         <v>688</v>
@@ -19668,7 +19724,7 @@
         <v>679</v>
       </c>
       <c r="I17" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J17">
         <v>25000</v>
@@ -19692,13 +19748,13 @@
         <v>25</v>
       </c>
       <c r="Q17" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R17" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S17" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T17">
         <v>40</v>
@@ -19710,7 +19766,7 @@
         <v>686</v>
       </c>
       <c r="W17" s="122" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="X17" s="122" t="s">
         <v>688</v>
@@ -19751,7 +19807,7 @@
         <v>679</v>
       </c>
       <c r="I18" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J18">
         <v>25000</v>
@@ -19775,13 +19831,13 @@
         <v>25</v>
       </c>
       <c r="Q18" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R18" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S18" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T18">
         <v>40</v>
@@ -19793,7 +19849,7 @@
         <v>686</v>
       </c>
       <c r="W18" s="122" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="X18" s="122" t="s">
         <v>688</v>
@@ -19858,7 +19914,7 @@
         <v>25</v>
       </c>
       <c r="Q19" s="122" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R19" s="122" t="s">
         <v>683</v>
@@ -19876,7 +19932,7 @@
         <v>686</v>
       </c>
       <c r="W19" s="122" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="X19" s="122" t="s">
         <v>688</v>
@@ -19917,7 +19973,7 @@
         <v>679</v>
       </c>
       <c r="I20" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J20">
         <v>25000</v>
@@ -19947,7 +20003,7 @@
         <v>131</v>
       </c>
       <c r="S20" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T20">
         <v>40</v>
@@ -19959,7 +20015,7 @@
         <v>686</v>
       </c>
       <c r="W20" s="122" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="X20" s="122" t="s">
         <v>688</v>
@@ -20000,7 +20056,7 @@
         <v>679</v>
       </c>
       <c r="I21" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J21">
         <v>25000</v>
@@ -20024,13 +20080,13 @@
         <v>25</v>
       </c>
       <c r="Q21" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R21" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S21" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T21">
         <v>40</v>
@@ -20042,7 +20098,7 @@
         <v>686</v>
       </c>
       <c r="W21" s="122" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="X21" s="122" t="s">
         <v>688</v>
@@ -20107,7 +20163,7 @@
         <v>25</v>
       </c>
       <c r="Q22" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R22" s="122" t="s">
         <v>683</v>
@@ -20125,7 +20181,7 @@
         <v>686</v>
       </c>
       <c r="W22" s="122" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="X22" s="122" t="s">
         <v>688</v>
@@ -20166,7 +20222,7 @@
         <v>679</v>
       </c>
       <c r="I23" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J23">
         <v>25000</v>
@@ -20190,13 +20246,13 @@
         <v>25</v>
       </c>
       <c r="Q23" s="122" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R23" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S23" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T23">
         <v>40</v>
@@ -20208,7 +20264,7 @@
         <v>686</v>
       </c>
       <c r="W23" s="122" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="X23" s="122" t="s">
         <v>688</v>
@@ -20237,7 +20293,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="222" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="F24" s="7">
         <v>25</v>
@@ -20249,7 +20305,7 @@
         <v>679</v>
       </c>
       <c r="I24" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J24">
         <v>25000</v>
@@ -20276,10 +20332,10 @@
         <v>682</v>
       </c>
       <c r="R24" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S24" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T24">
         <v>40</v>
@@ -20291,7 +20347,7 @@
         <v>686</v>
       </c>
       <c r="W24" s="122" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="X24" s="122" t="s">
         <v>688</v>
@@ -20320,7 +20376,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="222" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="F25" s="7">
         <v>25</v>
@@ -20356,7 +20412,7 @@
         <v>25</v>
       </c>
       <c r="Q25" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R25" s="122" t="s">
         <v>683</v>
@@ -20374,7 +20430,7 @@
         <v>686</v>
       </c>
       <c r="W25" s="122" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="X25" s="122" t="s">
         <v>688</v>
@@ -20403,7 +20459,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="222" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="F26" s="7">
         <v>25</v>
@@ -20415,7 +20471,7 @@
         <v>679</v>
       </c>
       <c r="I26" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J26">
         <v>25000</v>
@@ -20439,13 +20495,13 @@
         <v>25</v>
       </c>
       <c r="Q26" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R26" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S26" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T26">
         <v>40</v>
@@ -20457,7 +20513,7 @@
         <v>686</v>
       </c>
       <c r="W26" s="122" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="X26" s="122" t="s">
         <v>688</v>
@@ -20486,7 +20542,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="222" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="F27" s="7">
         <v>25</v>
@@ -20498,7 +20554,7 @@
         <v>679</v>
       </c>
       <c r="I27" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J27">
         <v>25000</v>
@@ -20522,13 +20578,13 @@
         <v>25</v>
       </c>
       <c r="Q27" s="122" t="s">
+        <v>1113</v>
+      </c>
+      <c r="R27" s="122" t="s">
         <v>1114</v>
       </c>
-      <c r="R27" s="122" t="s">
-        <v>1115</v>
-      </c>
       <c r="S27" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T27">
         <v>40</v>
@@ -20540,7 +20596,7 @@
         <v>686</v>
       </c>
       <c r="W27" s="122" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="X27" s="122" t="s">
         <v>688</v>
@@ -20569,7 +20625,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="222" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="F28" s="7">
         <v>25</v>
@@ -20623,7 +20679,7 @@
         <v>686</v>
       </c>
       <c r="W28" s="122" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="X28" s="122" t="s">
         <v>688</v>
@@ -20652,7 +20708,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="222" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="F29" s="7">
         <v>25</v>
@@ -20664,7 +20720,7 @@
         <v>679</v>
       </c>
       <c r="I29" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J29">
         <v>25000</v>
@@ -20688,13 +20744,13 @@
         <v>25</v>
       </c>
       <c r="Q29" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R29" s="122" t="s">
         <v>131</v>
       </c>
       <c r="S29" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T29">
         <v>40</v>
@@ -20706,7 +20762,7 @@
         <v>686</v>
       </c>
       <c r="W29" s="122" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="X29" s="122" t="s">
         <v>688</v>
@@ -20735,7 +20791,7 @@
         <v>3</v>
       </c>
       <c r="E30" s="222" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F30" s="7">
         <v>25</v>
@@ -20747,7 +20803,7 @@
         <v>679</v>
       </c>
       <c r="I30" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J30">
         <v>25000</v>
@@ -20771,13 +20827,13 @@
         <v>25</v>
       </c>
       <c r="Q30" s="122" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="R30" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S30" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T30">
         <v>40</v>
@@ -20789,7 +20845,7 @@
         <v>686</v>
       </c>
       <c r="W30" s="122" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="X30" s="122" t="s">
         <v>688</v>
@@ -20818,7 +20874,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="222" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="F31" s="7">
         <v>25</v>
@@ -20854,7 +20910,7 @@
         <v>25</v>
       </c>
       <c r="Q31" s="122" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="R31" s="122" t="s">
         <v>683</v>
@@ -20872,7 +20928,7 @@
         <v>686</v>
       </c>
       <c r="W31" s="122" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="X31" s="122" t="s">
         <v>688</v>
@@ -20913,7 +20969,7 @@
         <v>679</v>
       </c>
       <c r="I32" s="122" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="J32">
         <v>25000</v>
@@ -20943,7 +20999,7 @@
         <v>131</v>
       </c>
       <c r="S32" s="122" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="T32">
         <v>40</v>
@@ -20955,7 +21011,7 @@
         <v>686</v>
       </c>
       <c r="W32" s="122" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="X32" s="122" t="s">
         <v>688</v>
@@ -20984,7 +21040,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="222" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="F33" s="7">
         <v>25</v>
@@ -20996,7 +21052,7 @@
         <v>679</v>
       </c>
       <c r="I33" s="122" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="J33">
         <v>25000</v>
@@ -21020,13 +21076,13 @@
         <v>25</v>
       </c>
       <c r="Q33" s="122" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="R33" s="122" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="S33" s="122" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="T33">
         <v>40</v>
@@ -21038,7 +21094,7 @@
         <v>686</v>
       </c>
       <c r="W33" s="122" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="X33" s="122" t="s">
         <v>688</v>
@@ -21074,9 +21130,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG121"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W118" sqref="W118"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X116" sqref="X116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21303,7 +21359,7 @@
         <v>794</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -26886,7 +26942,7 @@
         <v>35</v>
       </c>
       <c r="I96" s="20"/>
-      <c r="L96" s="7" t="s">
+      <c r="J96" s="7" t="s">
         <v>35</v>
       </c>
       <c r="M96" s="82" t="s">
@@ -28000,9 +28056,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE134C92-48D1-46A0-9D4D-2C39D004BA3A}">
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC109" sqref="AC109"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30742,7 +30798,7 @@
         <v>224</v>
       </c>
       <c r="M84" s="97">
-        <v>1974570</v>
+        <v>1974579</v>
       </c>
       <c r="N84" t="s">
         <v>35</v>
@@ -31173,8 +31229,8 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O83" sqref="O83"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L102" sqref="L102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34598,9 +34654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H85" sqref="H85"/>
+      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34637,7 +34693,7 @@
         <v>217</v>
       </c>
       <c r="G1" s="166" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H1" s="166" t="s">
         <v>810</v>
@@ -36267,7 +36323,7 @@
         <v>35</v>
       </c>
       <c r="G80" s="158" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H80" s="64"/>
       <c r="I80" s="142" t="s">
@@ -36446,7 +36502,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37406,9 +37462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V83" sqref="V83"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W82" sqref="W82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37429,7 +37485,7 @@
     <col min="14" max="15" width="16" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
     <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.42578125" customWidth="1"/>
+    <col min="18" max="18" width="28" customWidth="1"/>
     <col min="19" max="19" width="10.7109375" customWidth="1"/>
     <col min="20" max="20" width="26.140625" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" customWidth="1"/>
@@ -39675,7 +39731,7 @@
         <v>8</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>621</v>
+        <v>1129</v>
       </c>
       <c r="N69" t="s">
         <v>224</v>
@@ -39710,7 +39766,7 @@
         <v>8</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>621</v>
+        <v>1130</v>
       </c>
       <c r="N70" t="s">
         <v>224</v>
@@ -39744,8 +39800,8 @@
       <c r="B71" s="7">
         <v>8</v>
       </c>
-      <c r="M71" s="2" t="s">
-        <v>621</v>
+      <c r="M71" s="230" t="s">
+        <v>1137</v>
       </c>
       <c r="N71" t="s">
         <v>224</v>
@@ -39780,7 +39836,7 @@
         <v>8</v>
       </c>
       <c r="M72" s="2" t="s">
-        <v>621</v>
+        <v>1136</v>
       </c>
       <c r="N72" t="s">
         <v>224</v>
@@ -39815,7 +39871,7 @@
         <v>8</v>
       </c>
       <c r="M73" s="2" t="s">
-        <v>621</v>
+        <v>1135</v>
       </c>
       <c r="N73" t="s">
         <v>224</v>
@@ -39850,7 +39906,7 @@
         <v>8</v>
       </c>
       <c r="M74" s="2" t="s">
-        <v>621</v>
+        <v>1134</v>
       </c>
       <c r="N74" t="s">
         <v>224</v>
@@ -39920,7 +39976,7 @@
         <v>8</v>
       </c>
       <c r="M76" s="2" t="s">
-        <v>621</v>
+        <v>1133</v>
       </c>
       <c r="N76" t="s">
         <v>224</v>
@@ -39955,7 +40011,7 @@
         <v>8</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>621</v>
+        <v>1132</v>
       </c>
       <c r="N77" t="s">
         <v>224</v>
@@ -40025,7 +40081,7 @@
         <v>8</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>621</v>
+        <v>1131</v>
       </c>
       <c r="N79" t="s">
         <v>224</v>
@@ -40059,6 +40115,7 @@
       <c r="B80" s="131">
         <v>8</v>
       </c>
+      <c r="S80" s="82"/>
       <c r="U80" s="100" t="s">
         <v>35</v>
       </c>
@@ -40076,6 +40133,9 @@
       <c r="N81" t="s">
         <v>224</v>
       </c>
+      <c r="S81" s="82">
+        <v>0</v>
+      </c>
       <c r="T81" s="104" t="s">
         <v>35</v>
       </c>
@@ -40093,6 +40153,9 @@
       <c r="N82" t="s">
         <v>224</v>
       </c>
+      <c r="S82" s="82">
+        <v>0</v>
+      </c>
       <c r="T82" s="104" t="s">
         <v>35</v>
       </c>
@@ -40110,6 +40173,9 @@
       <c r="N83" t="s">
         <v>224</v>
       </c>
+      <c r="S83" s="82">
+        <v>0</v>
+      </c>
       <c r="T83" s="104" t="s">
         <v>35</v>
       </c>
@@ -40127,6 +40193,9 @@
       <c r="N84" t="s">
         <v>224</v>
       </c>
+      <c r="S84" s="82">
+        <v>0</v>
+      </c>
       <c r="T84" s="104" t="s">
         <v>35</v>
       </c>
@@ -40144,6 +40213,9 @@
       <c r="N85" t="s">
         <v>224</v>
       </c>
+      <c r="S85" s="82">
+        <v>0</v>
+      </c>
       <c r="T85" s="104" t="s">
         <v>35</v>
       </c>
@@ -40161,6 +40233,9 @@
       <c r="N86" t="s">
         <v>224</v>
       </c>
+      <c r="S86" s="82">
+        <v>0</v>
+      </c>
       <c r="T86" s="104" t="s">
         <v>35</v>
       </c>
@@ -40177,6 +40252,9 @@
       </c>
       <c r="N87" t="s">
         <v>224</v>
+      </c>
+      <c r="S87" s="82">
+        <v>0</v>
       </c>
       <c r="T87" s="104" t="s">
         <v>35</v>
@@ -40196,8 +40274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40212,66 +40290,66 @@
     <col min="8" max="8" width="14.140625" style="4" customWidth="1"/>
     <col min="9" max="12" width="15.85546875" style="4" customWidth="1"/>
     <col min="13" max="14" width="15.140625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="4" customWidth="1"/>
     <col min="16" max="16" width="14" style="4" customWidth="1"/>
     <col min="17" max="17" width="17.140625" style="4" customWidth="1"/>
     <col min="18" max="18" width="16.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:18" s="229" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="93" t="s">
         <v>284</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="93" t="s">
         <v>285</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="93" t="s">
         <v>286</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="93" t="s">
         <v>287</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="93" t="s">
         <v>288</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="93" t="s">
         <v>289</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="228" t="s">
         <v>731</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="228" t="s">
         <v>243</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="228" t="s">
         <v>244</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="93" t="s">
         <v>291</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="93" t="s">
         <v>292</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="93" t="s">
         <v>293</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="93" t="s">
         <v>294</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="98" t="s">
         <v>295</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="98" t="s">
         <v>296</v>
       </c>
     </row>
@@ -40346,8 +40424,8 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="7">
-        <v>2000</v>
+      <c r="M3" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>

</xml_diff>

<commit_message>
fixed the url navigation issue
</commit_message>
<xml_diff>
--- a/resources/test_data/TestData_KLI.xlsx
+++ b/resources/test_data/TestData_KLI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praneethm\git\CodeLessFramework\resources\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF768C1-7962-4636-8CE4-465852EA2325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713BFF2E-4899-4059-8C4E-B9F83DA307B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="627" firstSheet="14" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="627" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogInPage" sheetId="22" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6029" uniqueCount="1215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6036" uniqueCount="1216">
   <si>
     <t>TestCaseNumber</t>
   </si>
@@ -3721,6 +3721,9 @@
   </si>
   <si>
     <t>PDFText&gt;Kotak e-Term Plan || A Pure Protection Plan || Premium Payment Term (in yrs) 41</t>
+  </si>
+  <si>
+    <t>PDFText&gt;Kotak e-Term Plan || A Pure Protection Plan || Premium Payment Term (in yrs) Single Premium</t>
   </si>
 </sst>
 </file>
@@ -5136,9 +5139,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5342,7 +5345,9 @@
       <c r="S3" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="51"/>
+      <c r="T3" s="51" t="s">
+        <v>31</v>
+      </c>
       <c r="U3" s="51" t="s">
         <v>31</v>
       </c>
@@ -5350,7 +5355,7 @@
         <v>154</v>
       </c>
       <c r="W3" s="51" t="s">
-        <v>29</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -12118,10 +12123,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12200,32 +12205,26 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>5010</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>318</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
-        <v>316</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>1974</v>
+      <c r="A4" s="2">
+        <v>5010</v>
       </c>
       <c r="B4" s="2">
         <v>10</v>
@@ -12248,17 +12247,17 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>1976</v>
+      <c r="A5" s="17">
+        <v>1974</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>541</v>
+        <v>317</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>542</v>
+        <v>318</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
@@ -12273,16 +12272,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B6" s="2">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -12297,16 +12296,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
-        <v>1981</v>
+        <v>1977</v>
       </c>
       <c r="B7" s="2">
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -12321,16 +12320,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="B8" s="2">
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
@@ -12345,16 +12344,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
@@ -12369,16 +12368,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
-        <v>1989</v>
+        <v>1985</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
@@ -12393,16 +12392,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -12417,16 +12416,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -12441,16 +12440,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -12465,16 +12464,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="B14" s="2">
         <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -12489,16 +12488,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B15" s="2">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -12513,80 +12512,80 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <v>3005</v>
-      </c>
-      <c r="B16" s="17">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+        <v>1999</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>562</v>
+      </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>316</v>
+      </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>717</v>
-      </c>
+      <c r="H16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>3005</v>
       </c>
-      <c r="B17" s="2">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1023</v>
-      </c>
+      <c r="B17" s="17">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>727</v>
-      </c>
+      <c r="H17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <v>3006</v>
+        <v>3005</v>
       </c>
       <c r="B18" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>562</v>
-      </c>
+        <v>1023</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>316</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="J18" s="2" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <v>3007</v>
+        <v>3006</v>
       </c>
       <c r="B19" s="2">
         <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>921</v>
+        <v>561</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>922</v>
+        <v>562</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
@@ -12601,16 +12600,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <v>3008</v>
+        <v>3007</v>
       </c>
       <c r="B20" s="2">
         <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
@@ -12625,16 +12624,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <v>3009</v>
+        <v>3008</v>
       </c>
       <c r="B21" s="2">
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
@@ -12649,16 +12648,16 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <v>3010</v>
+        <v>3009</v>
       </c>
       <c r="B22" s="2">
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
@@ -12673,16 +12672,16 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>3011</v>
+        <v>3010</v>
       </c>
       <c r="B23" s="2">
         <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
@@ -12694,6 +12693,30 @@
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>3011</v>
+      </c>
+      <c r="B24" s="2">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -12708,7 +12731,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17420,8 +17443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280E1A22-750B-4771-AF4C-76F857DCAC92}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17639,12 +17662,8 @@
       <c r="M5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
         <v>32</v>
       </c>
@@ -17721,12 +17740,8 @@
       <c r="M7" s="2">
         <v>0</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
       <c r="P7" s="2" t="s">
         <v>32</v>
       </c>
@@ -17891,12 +17906,8 @@
       <c r="M11" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
       <c r="P11" s="2" t="s">
         <v>32</v>
       </c>
@@ -18206,7 +18217,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19001,8 +19012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F83572-2E3E-46EC-A587-E2B7D9FD1095}">
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19232,7 +19243,9 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>645</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
@@ -21735,8 +21748,8 @@
   <dimension ref="A1:AJ131"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA81" sqref="AA81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26905,10 +26918,10 @@
       <c r="Z75" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AA75" s="2"/>
-      <c r="AB75" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="AA75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB75" s="2"/>
       <c r="AC75" s="2"/>
       <c r="AD75" s="2"/>
       <c r="AE75" s="2"/>
@@ -30613,8 +30626,8 @@
   <dimension ref="A1:Z118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30642,7 +30655,7 @@
     <col min="26" max="26" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="73" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="73" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -33064,7 +33077,7 @@
       </c>
       <c r="Z69" s="49"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>1971</v>
       </c>
@@ -33072,7 +33085,9 @@
       <c r="C70" s="50">
         <v>3</v>
       </c>
-      <c r="D70" s="49"/>
+      <c r="D70" s="49" t="s">
+        <v>199</v>
+      </c>
       <c r="E70" s="49"/>
       <c r="F70" s="49"/>
       <c r="G70" s="49"/>
@@ -33081,7 +33096,7 @@
       <c r="J70" s="49"/>
       <c r="K70" s="49"/>
       <c r="L70" s="49"/>
-      <c r="M70" s="49"/>
+      <c r="M70" s="66"/>
       <c r="N70" s="49"/>
       <c r="O70" s="49"/>
       <c r="P70" s="49"/>
@@ -34949,9 +34964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62E9860-6BD1-40AC-8E69-B88B9FD114A7}">
   <dimension ref="A1:AT104"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42849,7 +42864,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43954,9 +43969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Z85"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44148,7 +44163,9 @@
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="V3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="3"/>
@@ -44310,14 +44327,30 @@
       <c r="O7" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -47091,8 +47124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>